<commit_message>
agenda en planning aangepast
</commit_message>
<xml_diff>
--- a/Planning (PvA) en urenverantwoording/urenplanning en verantwoording.xlsx
+++ b/Planning (PvA) en urenverantwoording/urenplanning en verantwoording.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="65">
   <si>
     <t>Omschrijving activiteit</t>
   </si>
@@ -214,6 +214,9 @@
   </si>
   <si>
     <t>Vergaderen en notuleren</t>
+  </si>
+  <si>
+    <t>requirements architecture</t>
   </si>
 </sst>
 </file>
@@ -711,32 +714,32 @@
     <xf numFmtId="164" fontId="0" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1044,8 +1047,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O76"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" topLeftCell="C7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1073,18 +1076,18 @@
       <c r="D2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="104" t="s">
+      <c r="E2" s="106" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="104"/>
+      <c r="F2" s="106"/>
       <c r="H2" s="96" t="s">
         <v>54</v>
       </c>
-      <c r="I2" s="109">
+      <c r="I2" s="105">
         <f ca="1">TODAY()</f>
-        <v>42326</v>
-      </c>
-      <c r="J2" s="109"/>
+        <v>42331</v>
+      </c>
+      <c r="J2" s="105"/>
     </row>
     <row r="3" spans="1:15" s="1" customFormat="1" ht="83.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="56" t="s">
@@ -1136,26 +1139,26 @@
     <row r="4" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="16"/>
       <c r="B4" s="73"/>
-      <c r="D4" s="107" t="s">
+      <c r="D4" s="109" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="107"/>
-      <c r="F4" s="102" t="s">
+      <c r="E4" s="109"/>
+      <c r="F4" s="104" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="102"/>
-      <c r="H4" s="108" t="s">
+      <c r="G4" s="104"/>
+      <c r="H4" s="110" t="s">
         <v>12</v>
       </c>
-      <c r="I4" s="108"/>
-      <c r="J4" s="102" t="s">
+      <c r="I4" s="110"/>
+      <c r="J4" s="104" t="s">
         <v>13</v>
       </c>
-      <c r="K4" s="102"/>
-      <c r="L4" s="105" t="s">
-        <v>1</v>
-      </c>
-      <c r="M4" s="106"/>
+      <c r="K4" s="104"/>
+      <c r="L4" s="107" t="s">
+        <v>1</v>
+      </c>
+      <c r="M4" s="108"/>
       <c r="N4" s="22"/>
       <c r="O4" s="16"/>
     </row>
@@ -1171,8 +1174,8 @@
       <c r="G5" s="103"/>
       <c r="H5" s="103"/>
       <c r="I5" s="103"/>
-      <c r="J5" s="102"/>
-      <c r="K5" s="102"/>
+      <c r="J5" s="104"/>
+      <c r="K5" s="104"/>
       <c r="L5" s="94"/>
       <c r="M5" s="94"/>
       <c r="N5" s="95"/>
@@ -1407,10 +1410,10 @@
       <c r="G11" s="103"/>
       <c r="H11" s="103"/>
       <c r="I11" s="103"/>
-      <c r="J11" s="102" t="s">
+      <c r="J11" s="104" t="s">
         <v>39</v>
       </c>
-      <c r="K11" s="102"/>
+      <c r="K11" s="104"/>
       <c r="L11" s="94"/>
       <c r="M11" s="94"/>
       <c r="N11" s="95">
@@ -1646,7 +1649,7 @@
       <c r="B17" s="75">
         <v>42326</v>
       </c>
-      <c r="C17" s="110" t="s">
+      <c r="C17" s="102" t="s">
         <v>62</v>
       </c>
       <c r="D17" s="32">
@@ -1742,15 +1745,21 @@
       <c r="D19" s="32">
         <v>1.5</v>
       </c>
-      <c r="E19" s="32"/>
+      <c r="E19" s="32">
+        <v>1.5</v>
+      </c>
       <c r="F19" s="33">
         <v>1.5</v>
       </c>
-      <c r="G19" s="33"/>
+      <c r="G19" s="33">
+        <v>1.5</v>
+      </c>
       <c r="H19" s="34">
         <v>1</v>
       </c>
-      <c r="I19" s="34"/>
+      <c r="I19" s="34">
+        <v>1</v>
+      </c>
       <c r="J19" s="33"/>
       <c r="K19" s="33"/>
       <c r="L19" s="35"/>
@@ -1761,7 +1770,7 @@
       </c>
       <c r="O19" s="37">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -1783,7 +1792,9 @@
       <c r="J20" s="33">
         <v>3</v>
       </c>
-      <c r="K20" s="33"/>
+      <c r="K20" s="33">
+        <v>3</v>
+      </c>
       <c r="L20" s="35"/>
       <c r="M20" s="35"/>
       <c r="N20" s="36">
@@ -1792,7 +1803,7 @@
       </c>
       <c r="O20" s="37">
         <f t="shared" ref="O20:O21" si="12">E20+G20+I20+K20+M20</f>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -1808,19 +1819,27 @@
       <c r="D21" s="40">
         <v>0.25</v>
       </c>
-      <c r="E21" s="40"/>
+      <c r="E21" s="40">
+        <v>0.25</v>
+      </c>
       <c r="F21" s="62">
         <v>0.25</v>
       </c>
-      <c r="G21" s="62"/>
+      <c r="G21" s="62">
+        <v>0.25</v>
+      </c>
       <c r="H21" s="42">
         <v>0.25</v>
       </c>
-      <c r="I21" s="42"/>
+      <c r="I21" s="42">
+        <v>0.25</v>
+      </c>
       <c r="J21" s="41">
         <v>0.25</v>
       </c>
-      <c r="K21" s="41"/>
+      <c r="K21" s="41">
+        <v>0.25</v>
+      </c>
       <c r="L21" s="43"/>
       <c r="M21" s="43"/>
       <c r="N21" s="36">
@@ -1829,7 +1848,7 @@
       </c>
       <c r="O21" s="37">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -1844,10 +1863,10 @@
       <c r="G22" s="103"/>
       <c r="H22" s="103"/>
       <c r="I22" s="103"/>
-      <c r="J22" s="102" t="s">
+      <c r="J22" s="104" t="s">
         <v>47</v>
       </c>
-      <c r="K22" s="102"/>
+      <c r="K22" s="104"/>
       <c r="L22" s="94"/>
       <c r="M22" s="94"/>
       <c r="N22" s="95">
@@ -1856,7 +1875,7 @@
       </c>
       <c r="O22" s="95">
         <f>SUM(O12:O21)</f>
-        <v>30.25</v>
+        <v>38.25</v>
       </c>
     </row>
     <row r="23" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -2038,11 +2057,11 @@
       <c r="L27" s="59"/>
       <c r="M27" s="59"/>
       <c r="N27" s="36">
-        <f t="shared" ref="N27:N32" si="19">D27+F27+H27+J27+L27</f>
+        <f t="shared" ref="N27:N33" si="19">D27+F27+H27+J27+L27</f>
         <v>0.5</v>
       </c>
       <c r="O27" s="37">
-        <f t="shared" ref="O27:O32" si="20">E27+G27+I27+K27+M27</f>
+        <f t="shared" ref="O27:O33" si="20">E27+G27+I27+K27+M27</f>
         <v>0</v>
       </c>
     </row>
@@ -2050,7 +2069,9 @@
       <c r="A28" s="30">
         <v>3</v>
       </c>
-      <c r="B28" s="75"/>
+      <c r="B28" s="75">
+        <v>42331</v>
+      </c>
       <c r="C28" s="55" t="s">
         <v>32</v>
       </c>
@@ -2066,14 +2087,22 @@
       <c r="K28" s="37"/>
       <c r="L28" s="59"/>
       <c r="M28" s="59"/>
-      <c r="N28" s="36"/>
-      <c r="O28" s="37"/>
+      <c r="N28" s="36">
+        <f t="shared" ref="N28:N29" si="21">D28+F28+H28+J28+L28</f>
+        <v>0.25</v>
+      </c>
+      <c r="O28" s="37">
+        <f t="shared" ref="O28:O29" si="22">E28+G28+I28+K28+M28</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="29" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="30">
         <v>3</v>
       </c>
-      <c r="B29" s="75"/>
+      <c r="B29" s="75">
+        <v>42331</v>
+      </c>
       <c r="C29" s="55" t="s">
         <v>35</v>
       </c>
@@ -2089,8 +2118,14 @@
       <c r="K29" s="37"/>
       <c r="L29" s="59"/>
       <c r="M29" s="59"/>
-      <c r="N29" s="36"/>
-      <c r="O29" s="37"/>
+      <c r="N29" s="36">
+        <f t="shared" si="21"/>
+        <v>0.25</v>
+      </c>
+      <c r="O29" s="37">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="30" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="30">
@@ -2100,24 +2135,32 @@
         <v>42333</v>
       </c>
       <c r="C30" s="55" t="s">
-        <v>25</v>
-      </c>
-      <c r="D30" s="47"/>
+        <v>64</v>
+      </c>
+      <c r="D30" s="47">
+        <v>2</v>
+      </c>
       <c r="E30" s="47"/>
-      <c r="F30" s="37"/>
+      <c r="F30" s="37">
+        <v>2</v>
+      </c>
       <c r="G30" s="37"/>
-      <c r="H30" s="48"/>
+      <c r="H30" s="48">
+        <v>2</v>
+      </c>
       <c r="I30" s="48"/>
-      <c r="J30" s="37"/>
+      <c r="J30" s="37">
+        <v>2</v>
+      </c>
       <c r="K30" s="37"/>
       <c r="L30" s="46"/>
       <c r="M30" s="46"/>
       <c r="N30" s="36">
-        <f t="shared" si="19"/>
-        <v>0</v>
+        <f t="shared" ref="N30" si="23">D30+F30+H30+J30+L30</f>
+        <v>8</v>
       </c>
       <c r="O30" s="37">
-        <f t="shared" si="20"/>
+        <f t="shared" ref="O30" si="24">E30+G30+I30+K30+M30</f>
         <v>0</v>
       </c>
     </row>
@@ -2125,23 +2168,33 @@
       <c r="A31" s="30">
         <v>3</v>
       </c>
-      <c r="B31" s="75"/>
+      <c r="B31" s="75">
+        <v>42333</v>
+      </c>
       <c r="C31" s="55" t="s">
-        <v>31</v>
-      </c>
-      <c r="D31" s="47"/>
+        <v>25</v>
+      </c>
+      <c r="D31" s="47">
+        <v>2</v>
+      </c>
       <c r="E31" s="47"/>
-      <c r="F31" s="37"/>
+      <c r="F31" s="37">
+        <v>2</v>
+      </c>
       <c r="G31" s="37"/>
-      <c r="H31" s="48"/>
+      <c r="H31" s="48">
+        <v>2</v>
+      </c>
       <c r="I31" s="48"/>
-      <c r="J31" s="37"/>
+      <c r="J31" s="37">
+        <v>2</v>
+      </c>
       <c r="K31" s="37"/>
-      <c r="L31" s="49"/>
-      <c r="M31" s="49"/>
+      <c r="L31" s="46"/>
+      <c r="M31" s="46"/>
       <c r="N31" s="36">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="O31" s="37">
         <f t="shared" si="20"/>
@@ -2149,23 +2202,25 @@
       </c>
     </row>
     <row r="32" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="81">
+      <c r="A32" s="30">
         <v>3</v>
       </c>
-      <c r="B32" s="82"/>
+      <c r="B32" s="75">
+        <v>42334</v>
+      </c>
       <c r="C32" s="55" t="s">
-        <v>36</v>
-      </c>
-      <c r="D32" s="89"/>
-      <c r="E32" s="89"/>
-      <c r="F32" s="87"/>
-      <c r="G32" s="87"/>
-      <c r="H32" s="90"/>
-      <c r="I32" s="90"/>
-      <c r="J32" s="87"/>
-      <c r="K32" s="87"/>
-      <c r="L32" s="86"/>
-      <c r="M32" s="86"/>
+        <v>31</v>
+      </c>
+      <c r="D32" s="47"/>
+      <c r="E32" s="47"/>
+      <c r="F32" s="37"/>
+      <c r="G32" s="37"/>
+      <c r="H32" s="48"/>
+      <c r="I32" s="48"/>
+      <c r="J32" s="37"/>
+      <c r="K32" s="37"/>
+      <c r="L32" s="49"/>
+      <c r="M32" s="49"/>
       <c r="N32" s="36">
         <f t="shared" si="19"/>
         <v>0</v>
@@ -2176,111 +2231,95 @@
       </c>
     </row>
     <row r="33" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="38">
+      <c r="A33" s="81">
         <v>3</v>
       </c>
-      <c r="B33" s="76">
+      <c r="B33" s="82">
+        <v>42334</v>
+      </c>
+      <c r="C33" s="55" t="s">
+        <v>36</v>
+      </c>
+      <c r="D33" s="89"/>
+      <c r="E33" s="89"/>
+      <c r="F33" s="87"/>
+      <c r="G33" s="87"/>
+      <c r="H33" s="90"/>
+      <c r="I33" s="90"/>
+      <c r="J33" s="87"/>
+      <c r="K33" s="87"/>
+      <c r="L33" s="86"/>
+      <c r="M33" s="86"/>
+      <c r="N33" s="36">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="O33" s="37">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="38">
+        <v>3</v>
+      </c>
+      <c r="B34" s="76">
         <v>42337</v>
       </c>
-      <c r="C33" s="69" t="s">
+      <c r="C34" s="69" t="s">
         <v>30</v>
       </c>
-      <c r="D33" s="40">
-        <v>0.25</v>
-      </c>
-      <c r="E33" s="40"/>
-      <c r="F33" s="62">
-        <v>0.25</v>
-      </c>
-      <c r="G33" s="62"/>
-      <c r="H33" s="42">
-        <v>0.25</v>
-      </c>
-      <c r="I33" s="42"/>
-      <c r="J33" s="41">
-        <v>0.25</v>
-      </c>
-      <c r="K33" s="41"/>
-      <c r="L33" s="50"/>
-      <c r="M33" s="50"/>
-      <c r="N33" s="44">
-        <f t="shared" ref="N33:O33" si="21">D33+F33+H33+J33+L33</f>
-        <v>1</v>
-      </c>
-      <c r="O33" s="45">
-        <f t="shared" si="21"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="103" t="s">
+      <c r="D34" s="40">
+        <v>0.25</v>
+      </c>
+      <c r="E34" s="40"/>
+      <c r="F34" s="62">
+        <v>0.25</v>
+      </c>
+      <c r="G34" s="62"/>
+      <c r="H34" s="42">
+        <v>0.25</v>
+      </c>
+      <c r="I34" s="42"/>
+      <c r="J34" s="41">
+        <v>0.25</v>
+      </c>
+      <c r="K34" s="41"/>
+      <c r="L34" s="50"/>
+      <c r="M34" s="50"/>
+      <c r="N34" s="44">
+        <f t="shared" ref="N34:O34" si="25">D34+F34+H34+J34+L34</f>
+        <v>1</v>
+      </c>
+      <c r="O34" s="45">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="103" t="s">
         <v>42</v>
       </c>
-      <c r="B34" s="103"/>
-      <c r="C34" s="103"/>
-      <c r="D34" s="103"/>
-      <c r="E34" s="103"/>
-      <c r="F34" s="103"/>
-      <c r="G34" s="103"/>
-      <c r="H34" s="103"/>
-      <c r="I34" s="103"/>
-      <c r="J34" s="102" t="s">
+      <c r="B35" s="103"/>
+      <c r="C35" s="103"/>
+      <c r="D35" s="103"/>
+      <c r="E35" s="103"/>
+      <c r="F35" s="103"/>
+      <c r="G35" s="103"/>
+      <c r="H35" s="103"/>
+      <c r="I35" s="103"/>
+      <c r="J35" s="104" t="s">
         <v>48</v>
       </c>
-      <c r="K34" s="102"/>
-      <c r="L34" s="94"/>
-      <c r="M34" s="94"/>
-      <c r="N34" s="95">
-        <f>SUM(N23:N33)</f>
-        <v>18.5</v>
-      </c>
-      <c r="O34" s="95">
-        <f>SUM(O23:O33)</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="35" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="30">
-        <v>4</v>
-      </c>
-      <c r="B35" s="75">
-        <v>42338</v>
-      </c>
-      <c r="C35" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D35" s="47">
-        <v>2</v>
-      </c>
-      <c r="E35" s="47">
-        <v>2</v>
-      </c>
-      <c r="F35" s="37">
-        <v>2</v>
-      </c>
-      <c r="G35" s="37">
-        <v>2</v>
-      </c>
-      <c r="H35" s="48">
-        <v>2</v>
-      </c>
-      <c r="I35" s="48">
-        <v>2</v>
-      </c>
-      <c r="J35" s="37">
-        <v>2</v>
-      </c>
-      <c r="K35" s="37">
-        <v>2</v>
-      </c>
-      <c r="L35" s="58"/>
-      <c r="M35" s="58"/>
-      <c r="N35" s="28">
-        <f t="shared" ref="N35:N37" si="22">D35+F35+H35+J35+L35</f>
-        <v>8</v>
-      </c>
-      <c r="O35" s="37">
-        <f>E35+G35+I35+K35+M35</f>
+      <c r="K35" s="104"/>
+      <c r="L35" s="94"/>
+      <c r="M35" s="94"/>
+      <c r="N35" s="95">
+        <f>SUM(N23:N34)</f>
+        <v>35</v>
+      </c>
+      <c r="O35" s="95">
+        <f>SUM(O23:O34)</f>
         <v>8</v>
       </c>
     </row>
@@ -2313,11 +2352,11 @@
       <c r="L36" s="58"/>
       <c r="M36" s="58"/>
       <c r="N36" s="36">
-        <f t="shared" si="22"/>
+        <f t="shared" ref="N36:N37" si="26">D36+F36+H36+J36+L36</f>
         <v>2.5</v>
       </c>
       <c r="O36" s="37">
-        <f t="shared" ref="O36:O38" si="23">E36+G36+I36+K36+M36</f>
+        <f t="shared" ref="O36:O38" si="27">E36+G36+I36+K36+M36</f>
         <v>0</v>
       </c>
     </row>
@@ -2342,11 +2381,11 @@
       <c r="L37" s="46"/>
       <c r="M37" s="46"/>
       <c r="N37" s="36">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>0.25</v>
       </c>
       <c r="O37" s="37">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
     </row>
@@ -2375,7 +2414,7 @@
         <v>0</v>
       </c>
       <c r="O38" s="37">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
     </row>
@@ -2412,7 +2451,7 @@
         <v>2.5</v>
       </c>
       <c r="O39" s="37">
-        <f t="shared" ref="O39" si="24">E39+G39+I39+K39+M39</f>
+        <f t="shared" ref="O39" si="28">E39+G39+I39+K39+M39</f>
         <v>0</v>
       </c>
     </row>
@@ -2515,19 +2554,19 @@
       <c r="G43" s="103"/>
       <c r="H43" s="103"/>
       <c r="I43" s="103"/>
-      <c r="J43" s="102" t="s">
+      <c r="J43" s="104" t="s">
         <v>49</v>
       </c>
-      <c r="K43" s="102"/>
+      <c r="K43" s="104"/>
       <c r="L43" s="94"/>
       <c r="M43" s="94"/>
       <c r="N43" s="95">
-        <f>SUM(N35:N42)</f>
-        <v>14.25</v>
+        <f>SUM(N36:N42)</f>
+        <v>6.25</v>
       </c>
       <c r="O43" s="95">
-        <f>SUM(O35:O42)</f>
-        <v>8</v>
+        <f>SUM(O36:O42)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -2559,11 +2598,11 @@
       <c r="L44" s="46"/>
       <c r="M44" s="46"/>
       <c r="N44" s="28">
-        <f t="shared" ref="N44" si="25">D44+F44+H44+J44+L44</f>
+        <f t="shared" ref="N44" si="29">D44+F44+H44+J44+L44</f>
         <v>2.5</v>
       </c>
       <c r="O44" s="29">
-        <f t="shared" ref="O44" si="26">E44+G44+I44+K44+M44</f>
+        <f t="shared" ref="O44" si="30">E44+G44+I44+K44+M44</f>
         <v>0</v>
       </c>
     </row>
@@ -2588,11 +2627,11 @@
       <c r="L45" s="49"/>
       <c r="M45" s="49"/>
       <c r="N45" s="36">
-        <f t="shared" ref="N45" si="27">D45+F45+H45+J45+L45</f>
+        <f t="shared" ref="N45" si="31">D45+F45+H45+J45+L45</f>
         <v>0</v>
       </c>
       <c r="O45" s="37">
-        <f t="shared" ref="O45" si="28">E45+G45+I45+K45+M45</f>
+        <f t="shared" ref="O45" si="32">E45+G45+I45+K45+M45</f>
         <v>0</v>
       </c>
     </row>
@@ -2614,11 +2653,11 @@
       <c r="L46" s="49"/>
       <c r="M46" s="49"/>
       <c r="N46" s="36">
-        <f t="shared" ref="N46:O50" si="29">D46+F46+H46+J46+L46</f>
+        <f t="shared" ref="N46:O50" si="33">D46+F46+H46+J46+L46</f>
         <v>0</v>
       </c>
       <c r="O46" s="37">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
     </row>
@@ -2651,11 +2690,11 @@
       <c r="L47" s="49"/>
       <c r="M47" s="49"/>
       <c r="N47" s="36">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>2.5</v>
       </c>
       <c r="O47" s="37">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
     </row>
@@ -2678,11 +2717,11 @@
       <c r="L48" s="49"/>
       <c r="M48" s="49"/>
       <c r="N48" s="36">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="O48" s="37">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
     </row>
@@ -2703,11 +2742,11 @@
       <c r="L49" s="86"/>
       <c r="M49" s="86"/>
       <c r="N49" s="36">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="O49" s="37">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
     </row>
@@ -2740,11 +2779,11 @@
       <c r="L50" s="50"/>
       <c r="M50" s="50"/>
       <c r="N50" s="44">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>1</v>
       </c>
       <c r="O50" s="45">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
     </row>
@@ -2760,10 +2799,10 @@
       <c r="G51" s="103"/>
       <c r="H51" s="103"/>
       <c r="I51" s="103"/>
-      <c r="J51" s="102" t="s">
+      <c r="J51" s="104" t="s">
         <v>50</v>
       </c>
-      <c r="K51" s="102"/>
+      <c r="K51" s="104"/>
       <c r="L51" s="94"/>
       <c r="M51" s="94"/>
       <c r="N51" s="95">
@@ -2804,11 +2843,11 @@
       <c r="L52" s="46"/>
       <c r="M52" s="46"/>
       <c r="N52" s="28">
-        <f t="shared" ref="N52:O59" si="30">D52+F52+H52+J52+L52</f>
+        <f t="shared" ref="N52:O59" si="34">D52+F52+H52+J52+L52</f>
         <v>2.5</v>
       </c>
       <c r="O52" s="29">
-        <f t="shared" si="30"/>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
     </row>
@@ -2841,11 +2880,11 @@
       <c r="L53" s="98"/>
       <c r="M53" s="98"/>
       <c r="N53" s="99">
-        <f t="shared" ref="N53:N54" si="31">D53+F53+H53+J53+L53</f>
+        <f t="shared" ref="N53:N54" si="35">D53+F53+H53+J53+L53</f>
         <v>2.5</v>
       </c>
       <c r="O53" s="97">
-        <f t="shared" ref="O53:O54" si="32">E53+G53+I53+K53+M53</f>
+        <f t="shared" ref="O53:O54" si="36">E53+G53+I53+K53+M53</f>
         <v>0</v>
       </c>
     </row>
@@ -2868,11 +2907,11 @@
       <c r="L54" s="49"/>
       <c r="M54" s="49"/>
       <c r="N54" s="36">
-        <f t="shared" si="31"/>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="O54" s="37">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
     </row>
@@ -2893,11 +2932,11 @@
       <c r="L55" s="49"/>
       <c r="M55" s="49"/>
       <c r="N55" s="36">
-        <f t="shared" si="30"/>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="O55" s="37">
-        <f t="shared" si="30"/>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
     </row>
@@ -2918,11 +2957,11 @@
       <c r="L56" s="49"/>
       <c r="M56" s="49"/>
       <c r="N56" s="36">
-        <f t="shared" si="30"/>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="O56" s="37">
-        <f t="shared" si="30"/>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
     </row>
@@ -2943,11 +2982,11 @@
       <c r="L57" s="49"/>
       <c r="M57" s="49"/>
       <c r="N57" s="36">
-        <f t="shared" si="30"/>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="O57" s="37">
-        <f t="shared" si="30"/>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
     </row>
@@ -2968,11 +3007,11 @@
       <c r="L58" s="86"/>
       <c r="M58" s="86"/>
       <c r="N58" s="36">
-        <f t="shared" si="30"/>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="O58" s="37">
-        <f t="shared" si="30"/>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
     </row>
@@ -3005,11 +3044,11 @@
       <c r="L59" s="50"/>
       <c r="M59" s="50"/>
       <c r="N59" s="44">
-        <f t="shared" si="30"/>
+        <f t="shared" si="34"/>
         <v>1</v>
       </c>
       <c r="O59" s="45">
-        <f t="shared" si="30"/>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
     </row>
@@ -3028,7 +3067,7 @@
       <c r="J60" s="103" t="s">
         <v>51</v>
       </c>
-      <c r="K60" s="102"/>
+      <c r="K60" s="104"/>
       <c r="L60" s="94"/>
       <c r="M60" s="94"/>
       <c r="N60" s="95">
@@ -3069,11 +3108,11 @@
       <c r="L61" s="46"/>
       <c r="M61" s="46"/>
       <c r="N61" s="28">
-        <f t="shared" ref="N61:O66" si="33">D61+F61+H61+J61+L61</f>
+        <f t="shared" ref="N61:O66" si="37">D61+F61+H61+J61+L61</f>
         <v>2.5</v>
       </c>
       <c r="O61" s="29">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
     </row>
@@ -3106,11 +3145,11 @@
       <c r="L62" s="49"/>
       <c r="M62" s="49"/>
       <c r="N62" s="36">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>2.5</v>
       </c>
       <c r="O62" s="37">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
     </row>
@@ -3143,11 +3182,11 @@
       <c r="L63" s="49"/>
       <c r="M63" s="49"/>
       <c r="N63" s="36">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>2.5</v>
       </c>
       <c r="O63" s="37">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
     </row>
@@ -3180,11 +3219,11 @@
       <c r="L64" s="49"/>
       <c r="M64" s="49"/>
       <c r="N64" s="36">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>2.5</v>
       </c>
       <c r="O64" s="37">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
     </row>
@@ -3217,11 +3256,11 @@
       <c r="L65" s="49"/>
       <c r="M65" s="49"/>
       <c r="N65" s="36">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>2.5</v>
       </c>
       <c r="O65" s="37">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
     </row>
@@ -3242,11 +3281,11 @@
       <c r="L66" s="50"/>
       <c r="M66" s="50"/>
       <c r="N66" s="44">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="O66" s="45">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
     </row>
@@ -3265,7 +3304,7 @@
       <c r="J67" s="103" t="s">
         <v>52</v>
       </c>
-      <c r="K67" s="102"/>
+      <c r="K67" s="104"/>
       <c r="L67" s="94"/>
       <c r="M67" s="94"/>
       <c r="N67" s="95">
@@ -3306,11 +3345,11 @@
       <c r="L68" s="46"/>
       <c r="M68" s="46"/>
       <c r="N68" s="28">
-        <f t="shared" ref="N68:O70" si="34">D68+F68+H68+J68+L68</f>
+        <f t="shared" ref="N68:O70" si="38">D68+F68+H68+J68+L68</f>
         <v>2.5</v>
       </c>
       <c r="O68" s="29">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
     </row>
@@ -3343,11 +3382,11 @@
       <c r="L69" s="49"/>
       <c r="M69" s="49"/>
       <c r="N69" s="36">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>2.5</v>
       </c>
       <c r="O69" s="37">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
     </row>
@@ -3380,11 +3419,11 @@
       <c r="L70" s="49"/>
       <c r="M70" s="49"/>
       <c r="N70" s="36">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>2.5</v>
       </c>
       <c r="O70" s="37">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
     </row>
@@ -3417,11 +3456,11 @@
       <c r="L71" s="49"/>
       <c r="M71" s="49"/>
       <c r="N71" s="36">
-        <f t="shared" ref="N71:N74" si="35">D71+F71+H71+J71+L71</f>
+        <f t="shared" ref="N71:N74" si="39">D71+F71+H71+J71+L71</f>
         <v>2.5</v>
       </c>
       <c r="O71" s="37">
-        <f t="shared" ref="O71:O74" si="36">E71+G71+I71+K71+M71</f>
+        <f t="shared" ref="O71:O74" si="40">E71+G71+I71+K71+M71</f>
         <v>0</v>
       </c>
     </row>
@@ -3454,11 +3493,11 @@
       <c r="L72" s="49"/>
       <c r="M72" s="49"/>
       <c r="N72" s="36">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>2.5</v>
       </c>
       <c r="O72" s="37">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
     </row>
@@ -3479,11 +3518,11 @@
       <c r="L73" s="86"/>
       <c r="M73" s="86"/>
       <c r="N73" s="101">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="O73" s="87">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
     </row>
@@ -3506,11 +3545,11 @@
       <c r="L74" s="50"/>
       <c r="M74" s="50"/>
       <c r="N74" s="44">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="O74" s="45">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
     </row>
@@ -3527,7 +3566,7 @@
       <c r="J75" s="103" t="s">
         <v>53</v>
       </c>
-      <c r="K75" s="102"/>
+      <c r="K75" s="104"/>
       <c r="L75" s="2"/>
       <c r="M75" s="2"/>
       <c r="N75" s="8">
@@ -3546,48 +3585,48 @@
         <v>4</v>
       </c>
       <c r="D76" s="11">
-        <f>SUM(D4:D75)</f>
+        <f t="shared" ref="D76:M76" si="41">SUM(D4:D75)</f>
+        <v>33</v>
+      </c>
+      <c r="E76" s="11">
+        <f t="shared" si="41"/>
+        <v>19.5</v>
+      </c>
+      <c r="F76" s="11">
+        <f t="shared" si="41"/>
+        <v>41</v>
+      </c>
+      <c r="G76" s="11">
+        <f t="shared" si="41"/>
+        <v>19.25</v>
+      </c>
+      <c r="H76" s="11">
+        <f t="shared" si="41"/>
         <v>31</v>
       </c>
-      <c r="E76" s="11">
-        <f>SUM(E4:E75)</f>
-        <v>19.75</v>
-      </c>
-      <c r="F76" s="11">
-        <f>SUM(F4:F75)</f>
-        <v>39</v>
-      </c>
-      <c r="G76" s="11">
-        <f>SUM(G4:G75)</f>
-        <v>19.5</v>
-      </c>
-      <c r="H76" s="11">
-        <f>SUM(H4:H75)</f>
-        <v>29</v>
-      </c>
       <c r="I76" s="11">
-        <f>SUM(I4:I75)</f>
-        <v>19</v>
+        <f t="shared" si="41"/>
+        <v>18.25</v>
       </c>
       <c r="J76" s="11">
-        <f>SUM(J4:J75)</f>
-        <v>32</v>
+        <f t="shared" si="41"/>
+        <v>34</v>
       </c>
       <c r="K76" s="11">
-        <f>SUM(K4:K75)</f>
-        <v>19.5</v>
+        <f t="shared" si="41"/>
+        <v>20.75</v>
       </c>
       <c r="L76" s="11">
-        <f>SUM(L4:L75)</f>
+        <f t="shared" si="41"/>
         <v>0.5</v>
       </c>
       <c r="M76" s="11">
-        <f>SUM(M4:M75)</f>
+        <f t="shared" si="41"/>
         <v>0.5</v>
       </c>
       <c r="N76" s="9">
         <f>D76+F76+H76+J76+L76</f>
-        <v>131.5</v>
+        <v>139.5</v>
       </c>
       <c r="O76" s="11">
         <f>E76+G76+I76+K76+M76</f>
@@ -3596,6 +3635,14 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="A11:I11"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="J4:K4"/>
     <mergeCell ref="J75:K75"/>
     <mergeCell ref="I2:J2"/>
     <mergeCell ref="A5:I5"/>
@@ -3608,18 +3655,10 @@
     <mergeCell ref="J67:K67"/>
     <mergeCell ref="A22:I22"/>
     <mergeCell ref="J22:K22"/>
-    <mergeCell ref="A34:I34"/>
-    <mergeCell ref="J34:K34"/>
+    <mergeCell ref="A35:I35"/>
+    <mergeCell ref="J35:K35"/>
     <mergeCell ref="A43:I43"/>
     <mergeCell ref="J43:K43"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="A11:I11"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="L4:M4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="J4:K4"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.55118110236220474" right="0.55118110236220474" top="0.39370078740157483" bottom="0.39370078740157483" header="0.51181102362204722" footer="0.51181102362204722"/>
@@ -3645,20 +3684,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement>
-    <Volgorde_x0020_Documenten xmlns="9ab5e87a-ed8e-45a5-9793-059f67398425">6</Volgorde_x0020_Documenten>
-    <Categorie xmlns="9ab5e87a-ed8e-45a5-9793-059f67398425">Extra</Categorie>
-    <Week xmlns="9ab5e87a-ed8e-45a5-9793-059f67398425">Geen week</Week>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008D777D35650D3B43A23D41664AA30BC5" ma:contentTypeVersion="" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="7f80e5700d93aba1c148b391c267eb5e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9ab5e87a-ed8e-45a5-9793-059f67398425" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e36a552b910c1cdf142adc90bba5ebe9" ns2:_="">
     <xsd:import namespace="9ab5e87a-ed8e-45a5-9793-059f67398425"/>
@@ -3819,40 +3853,29 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+</file>
+
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement>
+    <Volgorde_x0020_Documenten xmlns="9ab5e87a-ed8e-45a5-9793-059f67398425">6</Volgorde_x0020_Documenten>
+    <Categorie xmlns="9ab5e87a-ed8e-45a5-9793-059f67398425">Extra</Categorie>
+    <Week xmlns="9ab5e87a-ed8e-45a5-9793-059f67398425">Geen week</Week>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D152C796-12D2-40E1-BE4C-837EB7333423}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7925AB61-19A0-4A39-BC21-6A09D18176D2}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="9ab5e87a-ed8e-45a5-9793-059f67398425"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1278A3E-47B6-4321-AA7E-C8551E08DBCA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C6B4BC2B-47EC-4A4E-997D-A663CFE6E409}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3870,10 +3893,26 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1278A3E-47B6-4321-AA7E-C8551E08DBCA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7925AB61-19A0-4A39-BC21-6A09D18176D2}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D152C796-12D2-40E1-BE4C-837EB7333423}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="9ab5e87a-ed8e-45a5-9793-059f67398425"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
uren en planning maar weer aangepast
</commit_message>
<xml_diff>
--- a/Planning (PvA) en urenverantwoording/urenplanning en verantwoording.xlsx
+++ b/Planning (PvA) en urenverantwoording/urenplanning en verantwoording.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="72">
   <si>
     <t>Omschrijving activiteit</t>
   </si>
@@ -226,6 +226,18 @@
   </si>
   <si>
     <t>PVA reviewpunten aanpassen</t>
+  </si>
+  <si>
+    <t>PVA reviewpunten aanpassen en laatste keer doorlezen</t>
+  </si>
+  <si>
+    <t>MoSCoW &amp; UCD</t>
+  </si>
+  <si>
+    <t>Planing maken voor komende 3 weken</t>
+  </si>
+  <si>
+    <t>RA verder afmaken</t>
   </si>
 </sst>
 </file>
@@ -729,28 +741,28 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1057,11 +1069,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O80"/>
+  <dimension ref="A1:O85"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K43" sqref="K43"/>
+      <pane ySplit="4" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1089,18 +1101,18 @@
       <c r="D2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="107" t="s">
+      <c r="E2" s="106" t="s">
         <v>63</v>
       </c>
-      <c r="F2" s="107"/>
+      <c r="F2" s="106"/>
       <c r="H2" s="96" t="s">
         <v>52</v>
       </c>
-      <c r="I2" s="106">
+      <c r="I2" s="111">
         <f ca="1">TODAY()</f>
-        <v>42341</v>
-      </c>
-      <c r="J2" s="106"/>
+        <v>42342</v>
+      </c>
+      <c r="J2" s="111"/>
     </row>
     <row r="3" spans="1:15" s="1" customFormat="1" ht="83.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="56" t="s">
@@ -1152,43 +1164,43 @@
     <row r="4" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="16"/>
       <c r="B4" s="73"/>
-      <c r="D4" s="110" t="s">
+      <c r="D4" s="109" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="110"/>
-      <c r="F4" s="105" t="s">
+      <c r="E4" s="109"/>
+      <c r="F4" s="104" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="105"/>
-      <c r="H4" s="111" t="s">
+      <c r="G4" s="104"/>
+      <c r="H4" s="110" t="s">
         <v>12</v>
       </c>
-      <c r="I4" s="111"/>
-      <c r="J4" s="105" t="s">
+      <c r="I4" s="110"/>
+      <c r="J4" s="104" t="s">
         <v>13</v>
       </c>
-      <c r="K4" s="105"/>
-      <c r="L4" s="108" t="s">
-        <v>1</v>
-      </c>
-      <c r="M4" s="109"/>
+      <c r="K4" s="104"/>
+      <c r="L4" s="107" t="s">
+        <v>1</v>
+      </c>
+      <c r="M4" s="108"/>
       <c r="N4" s="22"/>
       <c r="O4" s="16"/>
     </row>
     <row r="5" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="104" t="s">
+      <c r="A5" s="105" t="s">
         <v>38</v>
       </c>
-      <c r="B5" s="104"/>
-      <c r="C5" s="104"/>
-      <c r="D5" s="104"/>
-      <c r="E5" s="104"/>
-      <c r="F5" s="104"/>
-      <c r="G5" s="104"/>
-      <c r="H5" s="104"/>
-      <c r="I5" s="104"/>
-      <c r="J5" s="105"/>
-      <c r="K5" s="105"/>
+      <c r="B5" s="105"/>
+      <c r="C5" s="105"/>
+      <c r="D5" s="105"/>
+      <c r="E5" s="105"/>
+      <c r="F5" s="105"/>
+      <c r="G5" s="105"/>
+      <c r="H5" s="105"/>
+      <c r="I5" s="105"/>
+      <c r="J5" s="104"/>
+      <c r="K5" s="104"/>
       <c r="L5" s="94"/>
       <c r="M5" s="94"/>
       <c r="N5" s="95"/>
@@ -1412,21 +1424,21 @@
       </c>
     </row>
     <row r="11" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="104" t="s">
+      <c r="A11" s="105" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="104"/>
-      <c r="C11" s="104"/>
-      <c r="D11" s="104"/>
-      <c r="E11" s="104"/>
-      <c r="F11" s="104"/>
-      <c r="G11" s="104"/>
-      <c r="H11" s="104"/>
-      <c r="I11" s="104"/>
-      <c r="J11" s="105" t="s">
+      <c r="B11" s="105"/>
+      <c r="C11" s="105"/>
+      <c r="D11" s="105"/>
+      <c r="E11" s="105"/>
+      <c r="F11" s="105"/>
+      <c r="G11" s="105"/>
+      <c r="H11" s="105"/>
+      <c r="I11" s="105"/>
+      <c r="J11" s="104" t="s">
         <v>37</v>
       </c>
-      <c r="K11" s="105"/>
+      <c r="K11" s="104"/>
       <c r="L11" s="94"/>
       <c r="M11" s="94"/>
       <c r="N11" s="95">
@@ -1865,21 +1877,21 @@
       </c>
     </row>
     <row r="22" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="104" t="s">
+      <c r="A22" s="105" t="s">
         <v>39</v>
       </c>
-      <c r="B22" s="104"/>
-      <c r="C22" s="104"/>
-      <c r="D22" s="104"/>
-      <c r="E22" s="104"/>
-      <c r="F22" s="104"/>
-      <c r="G22" s="104"/>
-      <c r="H22" s="104"/>
-      <c r="I22" s="104"/>
-      <c r="J22" s="105" t="s">
+      <c r="B22" s="105"/>
+      <c r="C22" s="105"/>
+      <c r="D22" s="105"/>
+      <c r="E22" s="105"/>
+      <c r="F22" s="105"/>
+      <c r="G22" s="105"/>
+      <c r="H22" s="105"/>
+      <c r="I22" s="105"/>
+      <c r="J22" s="104" t="s">
         <v>45</v>
       </c>
-      <c r="K22" s="105"/>
+      <c r="K22" s="104"/>
       <c r="L22" s="94"/>
       <c r="M22" s="94"/>
       <c r="N22" s="95">
@@ -2399,21 +2411,21 @@
       </c>
     </row>
     <row r="36" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="104" t="s">
+      <c r="A36" s="105" t="s">
         <v>40</v>
       </c>
-      <c r="B36" s="104"/>
-      <c r="C36" s="104"/>
-      <c r="D36" s="104"/>
-      <c r="E36" s="104"/>
-      <c r="F36" s="104"/>
-      <c r="G36" s="104"/>
-      <c r="H36" s="104"/>
-      <c r="I36" s="104"/>
-      <c r="J36" s="105" t="s">
+      <c r="B36" s="105"/>
+      <c r="C36" s="105"/>
+      <c r="D36" s="105"/>
+      <c r="E36" s="105"/>
+      <c r="F36" s="105"/>
+      <c r="G36" s="105"/>
+      <c r="H36" s="105"/>
+      <c r="I36" s="105"/>
+      <c r="J36" s="104" t="s">
         <v>46</v>
       </c>
-      <c r="K36" s="105"/>
+      <c r="K36" s="104"/>
       <c r="L36" s="94"/>
       <c r="M36" s="94"/>
       <c r="N36" s="95">
@@ -2477,24 +2489,34 @@
       <c r="B38" s="75">
         <v>42338</v>
       </c>
-      <c r="C38" s="31"/>
+      <c r="C38" s="31" t="s">
+        <v>24</v>
+      </c>
       <c r="D38" s="47"/>
       <c r="E38" s="47"/>
-      <c r="F38" s="37"/>
-      <c r="G38" s="37"/>
+      <c r="F38" s="37">
+        <v>2</v>
+      </c>
+      <c r="G38" s="37">
+        <v>2</v>
+      </c>
       <c r="H38" s="48"/>
       <c r="I38" s="48"/>
-      <c r="J38" s="37"/>
-      <c r="K38" s="37"/>
+      <c r="J38" s="37">
+        <v>2</v>
+      </c>
+      <c r="K38" s="37">
+        <v>3</v>
+      </c>
       <c r="L38" s="103"/>
       <c r="M38" s="103"/>
       <c r="N38" s="36">
-        <f t="shared" ref="N38:N45" si="28">D38+F38+H38+J38+L38</f>
-        <v>0</v>
+        <f t="shared" ref="N38:N46" si="28">D38+F38+H38+J38+L38</f>
+        <v>4</v>
       </c>
       <c r="O38" s="37">
-        <f t="shared" ref="O38:O45" si="29">E38+G38+I38+K38+M38</f>
-        <v>0</v>
+        <f t="shared" ref="O38:O46" si="29">E38+G38+I38+K38+M38</f>
+        <v>5</v>
       </c>
     </row>
     <row r="39" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -2502,44 +2524,36 @@
         <v>4</v>
       </c>
       <c r="B39" s="75">
-        <v>42340</v>
-      </c>
-      <c r="C39" s="55" t="s">
-        <v>65</v>
+        <v>42338</v>
+      </c>
+      <c r="C39" s="31" t="s">
+        <v>69</v>
       </c>
       <c r="D39" s="47">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E39" s="47">
-        <v>1</v>
-      </c>
-      <c r="F39" s="37">
-        <v>1</v>
-      </c>
-      <c r="G39" s="37">
-        <v>1</v>
-      </c>
+        <v>2.5</v>
+      </c>
+      <c r="F39" s="37"/>
+      <c r="G39" s="37"/>
       <c r="H39" s="48">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I39" s="48">
-        <v>1</v>
-      </c>
-      <c r="J39" s="37">
-        <v>1</v>
-      </c>
-      <c r="K39" s="37">
-        <v>1</v>
-      </c>
-      <c r="L39" s="49"/>
-      <c r="M39" s="49"/>
+        <v>2</v>
+      </c>
+      <c r="J39" s="37"/>
+      <c r="K39" s="37"/>
+      <c r="L39" s="103"/>
+      <c r="M39" s="103"/>
       <c r="N39" s="36">
-        <f t="shared" si="28"/>
+        <f t="shared" ref="N39" si="30">D39+F39+H39+J39+L39</f>
         <v>4</v>
       </c>
       <c r="O39" s="37">
-        <f t="shared" si="29"/>
-        <v>4</v>
+        <f t="shared" ref="O39" si="31">E39+G39+I39+K39+M39</f>
+        <v>4.5</v>
       </c>
     </row>
     <row r="40" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -2550,13 +2564,13 @@
         <v>42340</v>
       </c>
       <c r="C40" s="55" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="D40" s="47">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E40" s="47">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="F40" s="37">
         <v>1</v>
@@ -2565,26 +2579,26 @@
         <v>1</v>
       </c>
       <c r="H40" s="48">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="I40" s="48">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J40" s="37">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="K40" s="37">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="L40" s="49"/>
       <c r="M40" s="49"/>
       <c r="N40" s="36">
         <f t="shared" si="28"/>
-        <v>2.5</v>
+        <v>4</v>
       </c>
       <c r="O40" s="37">
         <f t="shared" si="29"/>
-        <v>2.5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="41" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -2595,41 +2609,41 @@
         <v>42340</v>
       </c>
       <c r="C41" s="55" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D41" s="47">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="E41" s="47">
-        <v>1.5</v>
+        <v>0.5</v>
       </c>
       <c r="F41" s="37">
         <v>1</v>
       </c>
       <c r="G41" s="37">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="H41" s="48">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="I41" s="48">
-        <v>1.5</v>
+        <v>0.5</v>
       </c>
       <c r="J41" s="37">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="K41" s="37">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="L41" s="49"/>
       <c r="M41" s="49"/>
       <c r="N41" s="36">
         <f t="shared" si="28"/>
-        <v>5</v>
+        <v>2.5</v>
       </c>
       <c r="O41" s="37">
         <f t="shared" si="29"/>
-        <v>6.5</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="42" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -2637,44 +2651,44 @@
         <v>4</v>
       </c>
       <c r="B42" s="75">
-        <v>42341</v>
+        <v>42340</v>
       </c>
       <c r="C42" s="55" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D42" s="47">
+        <v>1</v>
+      </c>
+      <c r="E42" s="47">
         <v>1.5</v>
       </c>
-      <c r="E42" s="47">
-        <v>3</v>
-      </c>
       <c r="F42" s="37">
+        <v>1</v>
+      </c>
+      <c r="G42" s="37">
         <v>1.5</v>
       </c>
-      <c r="G42" s="37">
-        <v>3</v>
-      </c>
       <c r="H42" s="48">
+        <v>1</v>
+      </c>
+      <c r="I42" s="48">
         <v>1.5</v>
       </c>
-      <c r="I42" s="48">
-        <v>1</v>
-      </c>
       <c r="J42" s="37">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="K42" s="37">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="L42" s="49"/>
       <c r="M42" s="49"/>
       <c r="N42" s="36">
         <f t="shared" si="28"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="O42" s="37">
         <f t="shared" si="29"/>
-        <v>8.5</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="43" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -2682,36 +2696,44 @@
         <v>4</v>
       </c>
       <c r="B43" s="75">
-        <v>42342</v>
+        <v>42341</v>
       </c>
       <c r="C43" s="55" t="s">
         <v>67</v>
       </c>
       <c r="D43" s="47">
-        <v>1</v>
-      </c>
-      <c r="E43" s="47"/>
+        <v>1.5</v>
+      </c>
+      <c r="E43" s="47">
+        <v>3</v>
+      </c>
       <c r="F43" s="37">
-        <v>1</v>
-      </c>
-      <c r="G43" s="37"/>
+        <v>1.5</v>
+      </c>
+      <c r="G43" s="37">
+        <v>3</v>
+      </c>
       <c r="H43" s="48">
-        <v>1</v>
-      </c>
-      <c r="I43" s="48"/>
+        <v>1.5</v>
+      </c>
+      <c r="I43" s="48">
+        <v>1</v>
+      </c>
       <c r="J43" s="37">
-        <v>1</v>
-      </c>
-      <c r="K43" s="37"/>
+        <v>1.5</v>
+      </c>
+      <c r="K43" s="37">
+        <v>1.5</v>
+      </c>
       <c r="L43" s="49"/>
       <c r="M43" s="49"/>
       <c r="N43" s="36">
         <f t="shared" si="28"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="O43" s="37">
         <f t="shared" si="29"/>
-        <v>0</v>
+        <v>8.5</v>
       </c>
     </row>
     <row r="44" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -2721,189 +2743,199 @@
       <c r="B44" s="75">
         <v>42342</v>
       </c>
-      <c r="C44" s="31" t="s">
-        <v>23</v>
+      <c r="C44" s="55" t="s">
+        <v>68</v>
       </c>
       <c r="D44" s="47">
-        <v>0.25</v>
-      </c>
-      <c r="E44" s="47"/>
-      <c r="F44" s="37"/>
-      <c r="G44" s="37"/>
-      <c r="H44" s="48"/>
-      <c r="I44" s="48"/>
-      <c r="J44" s="37"/>
-      <c r="K44" s="37"/>
+        <v>1</v>
+      </c>
+      <c r="E44" s="47">
+        <v>2.5</v>
+      </c>
+      <c r="F44" s="37">
+        <v>1</v>
+      </c>
+      <c r="G44" s="37">
+        <v>1</v>
+      </c>
+      <c r="H44" s="48">
+        <v>1</v>
+      </c>
+      <c r="I44" s="48">
+        <v>0</v>
+      </c>
+      <c r="J44" s="37">
+        <v>1</v>
+      </c>
+      <c r="K44" s="37">
+        <v>0.5</v>
+      </c>
       <c r="L44" s="49"/>
       <c r="M44" s="49"/>
       <c r="N44" s="36">
         <f t="shared" si="28"/>
-        <v>0.25</v>
+        <v>4</v>
       </c>
       <c r="O44" s="37">
         <f t="shared" si="29"/>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="45" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="81">
+      <c r="A45" s="30">
         <v>4</v>
       </c>
-      <c r="B45" s="82"/>
-      <c r="C45" s="83"/>
-      <c r="D45" s="89"/>
-      <c r="E45" s="89"/>
-      <c r="F45" s="87"/>
-      <c r="G45" s="87"/>
-      <c r="H45" s="90"/>
-      <c r="I45" s="90"/>
-      <c r="J45" s="87"/>
-      <c r="K45" s="87"/>
-      <c r="L45" s="86"/>
-      <c r="M45" s="86"/>
+      <c r="B45" s="75">
+        <v>42342</v>
+      </c>
+      <c r="C45" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="D45" s="47">
+        <v>0.25</v>
+      </c>
+      <c r="E45" s="47">
+        <v>0.25</v>
+      </c>
+      <c r="F45" s="37"/>
+      <c r="G45" s="37"/>
+      <c r="H45" s="48"/>
+      <c r="I45" s="48"/>
+      <c r="J45" s="37"/>
+      <c r="K45" s="37"/>
+      <c r="L45" s="49"/>
+      <c r="M45" s="49"/>
       <c r="N45" s="36">
         <f t="shared" si="28"/>
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="O45" s="37">
         <f t="shared" si="29"/>
-        <v>0</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="46" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="38">
+      <c r="A46" s="81">
         <v>4</v>
       </c>
-      <c r="B46" s="76">
+      <c r="B46" s="82"/>
+      <c r="C46" s="83"/>
+      <c r="D46" s="89"/>
+      <c r="E46" s="89"/>
+      <c r="F46" s="87"/>
+      <c r="G46" s="87"/>
+      <c r="H46" s="90"/>
+      <c r="I46" s="90"/>
+      <c r="J46" s="87"/>
+      <c r="K46" s="87"/>
+      <c r="L46" s="86"/>
+      <c r="M46" s="86"/>
+      <c r="N46" s="36">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="O46" s="37">
+        <f t="shared" si="29"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="38">
+        <v>4</v>
+      </c>
+      <c r="B47" s="76">
         <v>42344</v>
       </c>
-      <c r="C46" s="69" t="s">
+      <c r="C47" s="69" t="s">
         <v>29</v>
       </c>
-      <c r="D46" s="40">
-        <v>0.25</v>
-      </c>
-      <c r="E46" s="40"/>
-      <c r="F46" s="62">
-        <v>0.25</v>
-      </c>
-      <c r="G46" s="62"/>
-      <c r="H46" s="42">
-        <v>0.25</v>
-      </c>
-      <c r="I46" s="42"/>
-      <c r="J46" s="41">
-        <v>0.25</v>
-      </c>
-      <c r="K46" s="41"/>
-      <c r="L46" s="50"/>
-      <c r="M46" s="50"/>
-      <c r="N46" s="44">
-        <f>D46+F46+H46+J46+L46</f>
-        <v>1</v>
-      </c>
-      <c r="O46" s="45">
-        <f>E46+G46+I46+K46+M46</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="104" t="s">
+      <c r="D47" s="40">
+        <v>0.25</v>
+      </c>
+      <c r="E47" s="40"/>
+      <c r="F47" s="62">
+        <v>0.25</v>
+      </c>
+      <c r="G47" s="62"/>
+      <c r="H47" s="42">
+        <v>0.25</v>
+      </c>
+      <c r="I47" s="42"/>
+      <c r="J47" s="41">
+        <v>0.25</v>
+      </c>
+      <c r="K47" s="41"/>
+      <c r="L47" s="50"/>
+      <c r="M47" s="50"/>
+      <c r="N47" s="44">
+        <f>D47+F47+H47+J47+L47</f>
+        <v>1</v>
+      </c>
+      <c r="O47" s="45">
+        <f>E47+G47+I47+K47+M47</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="105" t="s">
         <v>41</v>
       </c>
-      <c r="B47" s="104"/>
-      <c r="C47" s="104"/>
-      <c r="D47" s="104"/>
-      <c r="E47" s="104"/>
-      <c r="F47" s="104"/>
-      <c r="G47" s="104"/>
-      <c r="H47" s="104"/>
-      <c r="I47" s="104"/>
-      <c r="J47" s="105" t="s">
+      <c r="B48" s="105"/>
+      <c r="C48" s="105"/>
+      <c r="D48" s="105"/>
+      <c r="E48" s="105"/>
+      <c r="F48" s="105"/>
+      <c r="G48" s="105"/>
+      <c r="H48" s="105"/>
+      <c r="I48" s="105"/>
+      <c r="J48" s="104" t="s">
         <v>47</v>
       </c>
-      <c r="K47" s="105"/>
-      <c r="L47" s="94"/>
-      <c r="M47" s="94"/>
-      <c r="N47" s="95">
-        <f>SUM(N37:N46)</f>
-        <v>24.75</v>
-      </c>
-      <c r="O47" s="95">
-        <f>SUM(O37:O46)</f>
-        <v>26</v>
-      </c>
-    </row>
-    <row r="48" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="23">
+      <c r="K48" s="104"/>
+      <c r="L48" s="94"/>
+      <c r="M48" s="94"/>
+      <c r="N48" s="95">
+        <f>SUM(N37:N47)</f>
+        <v>32.75</v>
+      </c>
+      <c r="O48" s="95">
+        <f>SUM(O37:O47)</f>
+        <v>39.75</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="23">
         <v>4</v>
       </c>
-      <c r="B48" s="74">
+      <c r="B49" s="74">
         <v>42345</v>
       </c>
-      <c r="C48" s="57" t="s">
+      <c r="C49" s="57" t="s">
         <v>61</v>
       </c>
-      <c r="D48" s="47">
-        <v>0.5</v>
-      </c>
-      <c r="E48" s="47"/>
-      <c r="F48" s="37">
-        <v>1</v>
-      </c>
-      <c r="G48" s="37"/>
-      <c r="H48" s="48">
-        <v>0.5</v>
-      </c>
-      <c r="I48" s="48"/>
-      <c r="J48" s="37">
-        <v>0.5</v>
-      </c>
-      <c r="K48" s="29"/>
-      <c r="L48" s="46"/>
-      <c r="M48" s="46"/>
-      <c r="N48" s="28">
-        <f t="shared" ref="N48" si="30">D48+F48+H48+J48+L48</f>
-        <v>2.5</v>
-      </c>
-      <c r="O48" s="29">
-        <f t="shared" ref="O48" si="31">E48+G48+I48+K48+M48</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="30">
-        <v>5</v>
-      </c>
-      <c r="B49" s="75">
-        <v>42345</v>
-      </c>
-      <c r="C49" s="55" t="s">
-        <v>32</v>
-      </c>
       <c r="D49" s="47">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E49" s="47"/>
       <c r="F49" s="37">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G49" s="37"/>
       <c r="H49" s="48">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I49" s="48"/>
       <c r="J49" s="37">
-        <v>2</v>
-      </c>
-      <c r="K49" s="37"/>
-      <c r="L49" s="49"/>
-      <c r="M49" s="49"/>
-      <c r="N49" s="36">
+        <v>0</v>
+      </c>
+      <c r="K49" s="29"/>
+      <c r="L49" s="46"/>
+      <c r="M49" s="46"/>
+      <c r="N49" s="28">
         <f t="shared" ref="N49" si="32">D49+F49+H49+J49+L49</f>
-        <v>8</v>
-      </c>
-      <c r="O49" s="37">
+        <v>0</v>
+      </c>
+      <c r="O49" s="29">
         <f t="shared" ref="O49" si="33">E49+G49+I49+K49+M49</f>
         <v>0</v>
       </c>
@@ -2915,22 +2947,33 @@
       <c r="B50" s="75">
         <v>42345</v>
       </c>
-      <c r="D50" s="47"/>
+      <c r="C50" s="55" t="s">
+        <v>32</v>
+      </c>
+      <c r="D50" s="47">
+        <v>2</v>
+      </c>
       <c r="E50" s="47"/>
-      <c r="F50" s="37"/>
+      <c r="F50" s="37">
+        <v>2</v>
+      </c>
       <c r="G50" s="37"/>
-      <c r="H50" s="48"/>
+      <c r="H50" s="48">
+        <v>2</v>
+      </c>
       <c r="I50" s="48"/>
-      <c r="J50" s="37"/>
+      <c r="J50" s="37">
+        <v>2</v>
+      </c>
       <c r="K50" s="37"/>
       <c r="L50" s="49"/>
       <c r="M50" s="49"/>
       <c r="N50" s="36">
-        <f t="shared" ref="N50:O54" si="34">D50+F50+H50+J50+L50</f>
-        <v>0</v>
+        <f t="shared" ref="N50" si="34">D50+F50+H50+J50+L50</f>
+        <v>8</v>
       </c>
       <c r="O50" s="37">
-        <f t="shared" si="34"/>
+        <f t="shared" ref="O50" si="35">E50+G50+I50+K50+M50</f>
         <v>0</v>
       </c>
     </row>
@@ -2939,35 +2982,35 @@
         <v>5</v>
       </c>
       <c r="B51" s="75">
-        <v>42347</v>
+        <v>42345</v>
       </c>
       <c r="C51" s="55" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="D51" s="47">
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="E51" s="47"/>
       <c r="F51" s="37">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G51" s="37"/>
       <c r="H51" s="48">
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="I51" s="48"/>
       <c r="J51" s="37">
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="K51" s="37"/>
       <c r="L51" s="49"/>
       <c r="M51" s="49"/>
       <c r="N51" s="36">
-        <f t="shared" si="34"/>
-        <v>2.5</v>
+        <f t="shared" ref="N51:N57" si="36">D51+F51+H51+J51+L51</f>
+        <v>8</v>
       </c>
       <c r="O51" s="37">
-        <f t="shared" si="34"/>
+        <f t="shared" ref="O51:O57" si="37">E51+G51+I51+K51+M51</f>
         <v>0</v>
       </c>
     </row>
@@ -2975,13 +3018,11 @@
       <c r="A52" s="30">
         <v>5</v>
       </c>
-      <c r="B52" s="75"/>
-      <c r="C52" s="55" t="s">
-        <v>35</v>
-      </c>
-      <c r="D52" s="47">
-        <v>0.25</v>
-      </c>
+      <c r="B52" s="75">
+        <v>42345</v>
+      </c>
+      <c r="C52" s="55"/>
+      <c r="D52" s="47"/>
       <c r="E52" s="47"/>
       <c r="F52" s="37"/>
       <c r="G52" s="37"/>
@@ -2992,111 +3033,123 @@
       <c r="L52" s="49"/>
       <c r="M52" s="49"/>
       <c r="N52" s="36">
-        <f t="shared" si="34"/>
-        <v>0.25</v>
+        <f t="shared" si="36"/>
+        <v>0</v>
       </c>
       <c r="O52" s="37">
-        <f t="shared" si="34"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="81">
+      <c r="A53" s="30">
         <v>5</v>
       </c>
-      <c r="B53" s="82"/>
-      <c r="C53" s="88"/>
-      <c r="D53" s="89"/>
-      <c r="E53" s="89"/>
-      <c r="F53" s="87"/>
-      <c r="G53" s="87"/>
-      <c r="H53" s="90"/>
-      <c r="I53" s="90"/>
-      <c r="J53" s="87"/>
-      <c r="K53" s="87"/>
-      <c r="L53" s="86"/>
-      <c r="M53" s="86"/>
+      <c r="B53" s="75">
+        <v>42345</v>
+      </c>
+      <c r="C53" s="55"/>
+      <c r="D53" s="47"/>
+      <c r="E53" s="47"/>
+      <c r="F53" s="37"/>
+      <c r="G53" s="37"/>
+      <c r="H53" s="48"/>
+      <c r="I53" s="48"/>
+      <c r="J53" s="37"/>
+      <c r="K53" s="37"/>
+      <c r="L53" s="49"/>
+      <c r="M53" s="49"/>
       <c r="N53" s="36">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="O53" s="37">
-        <f t="shared" si="34"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="38">
+      <c r="A54" s="30">
         <v>5</v>
       </c>
-      <c r="B54" s="76">
-        <v>42351</v>
-      </c>
-      <c r="C54" s="69" t="s">
-        <v>29</v>
-      </c>
-      <c r="D54" s="40">
-        <v>0.25</v>
-      </c>
-      <c r="E54" s="40"/>
-      <c r="F54" s="62">
-        <v>0.25</v>
-      </c>
-      <c r="G54" s="62"/>
-      <c r="H54" s="42">
-        <v>0.25</v>
-      </c>
-      <c r="I54" s="42"/>
-      <c r="J54" s="41">
-        <v>0.25</v>
-      </c>
-      <c r="K54" s="41"/>
-      <c r="L54" s="50"/>
-      <c r="M54" s="50"/>
-      <c r="N54" s="44">
-        <f t="shared" si="34"/>
-        <v>1</v>
-      </c>
-      <c r="O54" s="45">
-        <f t="shared" si="34"/>
+      <c r="B54" s="75">
+        <v>42347</v>
+      </c>
+      <c r="C54" s="55" t="s">
+        <v>34</v>
+      </c>
+      <c r="D54" s="47">
+        <v>1</v>
+      </c>
+      <c r="E54" s="47"/>
+      <c r="F54" s="37">
+        <v>1</v>
+      </c>
+      <c r="G54" s="37"/>
+      <c r="H54" s="48">
+        <v>1</v>
+      </c>
+      <c r="I54" s="48"/>
+      <c r="J54" s="37">
+        <v>1</v>
+      </c>
+      <c r="K54" s="37"/>
+      <c r="L54" s="49"/>
+      <c r="M54" s="49"/>
+      <c r="N54" s="36">
+        <f t="shared" si="36"/>
+        <v>4</v>
+      </c>
+      <c r="O54" s="37">
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="104" t="s">
-        <v>42</v>
-      </c>
-      <c r="B55" s="104"/>
-      <c r="C55" s="104"/>
-      <c r="D55" s="104"/>
-      <c r="E55" s="104"/>
-      <c r="F55" s="104"/>
-      <c r="G55" s="104"/>
-      <c r="H55" s="104"/>
-      <c r="I55" s="104"/>
-      <c r="J55" s="105" t="s">
-        <v>48</v>
-      </c>
-      <c r="K55" s="105"/>
-      <c r="L55" s="94"/>
-      <c r="M55" s="94"/>
-      <c r="N55" s="95">
-        <f>SUM(N48:N54)</f>
-        <v>14.25</v>
-      </c>
-      <c r="O55" s="95">
-        <f>SUM(O48:O54)</f>
+      <c r="A55" s="30">
+        <v>5</v>
+      </c>
+      <c r="B55" s="75">
+        <v>42347</v>
+      </c>
+      <c r="C55" s="55" t="s">
+        <v>70</v>
+      </c>
+      <c r="D55" s="47">
+        <v>0.25</v>
+      </c>
+      <c r="E55" s="47"/>
+      <c r="F55" s="37">
+        <v>0.25</v>
+      </c>
+      <c r="G55" s="37"/>
+      <c r="H55" s="48">
+        <v>0.25</v>
+      </c>
+      <c r="I55" s="48"/>
+      <c r="J55" s="37">
+        <v>0.25</v>
+      </c>
+      <c r="K55" s="37"/>
+      <c r="L55" s="49"/>
+      <c r="M55" s="49"/>
+      <c r="N55" s="36">
+        <f t="shared" si="36"/>
+        <v>1</v>
+      </c>
+      <c r="O55" s="37">
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="23">
-        <v>6</v>
-      </c>
-      <c r="B56" s="74">
-        <v>42352</v>
-      </c>
-      <c r="C56" s="92" t="s">
+      <c r="A56" s="30">
+        <v>5</v>
+      </c>
+      <c r="B56" s="75">
+        <v>42347</v>
+      </c>
+      <c r="C56" s="55" t="s">
         <v>61</v>
       </c>
       <c r="D56" s="47">
@@ -3114,491 +3167,485 @@
       <c r="J56" s="37">
         <v>0.5</v>
       </c>
-      <c r="K56" s="29"/>
-      <c r="L56" s="46"/>
-      <c r="M56" s="46"/>
-      <c r="N56" s="28">
-        <f t="shared" ref="N56:O63" si="35">D56+F56+H56+J56+L56</f>
+      <c r="K56" s="37"/>
+      <c r="L56" s="49"/>
+      <c r="M56" s="49"/>
+      <c r="N56" s="36">
+        <f t="shared" si="36"/>
         <v>2.5</v>
       </c>
-      <c r="O56" s="29">
-        <f t="shared" si="35"/>
+      <c r="O56" s="37">
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="64">
+      <c r="A57" s="30">
+        <v>5</v>
+      </c>
+      <c r="B57" s="75">
+        <v>42347</v>
+      </c>
+      <c r="C57" s="55" t="s">
+        <v>35</v>
+      </c>
+      <c r="D57" s="47">
+        <v>0.25</v>
+      </c>
+      <c r="E57" s="47"/>
+      <c r="F57" s="37"/>
+      <c r="G57" s="37"/>
+      <c r="H57" s="48"/>
+      <c r="I57" s="48"/>
+      <c r="J57" s="37"/>
+      <c r="K57" s="37"/>
+      <c r="L57" s="49"/>
+      <c r="M57" s="49"/>
+      <c r="N57" s="36">
+        <f t="shared" si="36"/>
+        <v>0.25</v>
+      </c>
+      <c r="O57" s="37">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="81">
+        <v>5</v>
+      </c>
+      <c r="B58" s="82"/>
+      <c r="C58" s="88"/>
+      <c r="D58" s="89"/>
+      <c r="E58" s="89"/>
+      <c r="F58" s="87"/>
+      <c r="G58" s="87"/>
+      <c r="H58" s="90"/>
+      <c r="I58" s="90"/>
+      <c r="J58" s="87"/>
+      <c r="K58" s="87"/>
+      <c r="L58" s="86"/>
+      <c r="M58" s="86"/>
+      <c r="N58" s="36">
+        <f t="shared" ref="N56:O59" si="38">D58+F58+H58+J58+L58</f>
+        <v>0</v>
+      </c>
+      <c r="O58" s="37">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="38">
+        <v>5</v>
+      </c>
+      <c r="B59" s="76">
+        <v>42351</v>
+      </c>
+      <c r="C59" s="69" t="s">
+        <v>29</v>
+      </c>
+      <c r="D59" s="40">
+        <v>0.25</v>
+      </c>
+      <c r="E59" s="40"/>
+      <c r="F59" s="62">
+        <v>0.25</v>
+      </c>
+      <c r="G59" s="62"/>
+      <c r="H59" s="42">
+        <v>0.25</v>
+      </c>
+      <c r="I59" s="42"/>
+      <c r="J59" s="41">
+        <v>0.25</v>
+      </c>
+      <c r="K59" s="41"/>
+      <c r="L59" s="50"/>
+      <c r="M59" s="50"/>
+      <c r="N59" s="44">
+        <f t="shared" si="38"/>
+        <v>1</v>
+      </c>
+      <c r="O59" s="45">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="105" t="s">
+        <v>42</v>
+      </c>
+      <c r="B60" s="105"/>
+      <c r="C60" s="105"/>
+      <c r="D60" s="105"/>
+      <c r="E60" s="105"/>
+      <c r="F60" s="105"/>
+      <c r="G60" s="105"/>
+      <c r="H60" s="105"/>
+      <c r="I60" s="105"/>
+      <c r="J60" s="104" t="s">
+        <v>48</v>
+      </c>
+      <c r="K60" s="104"/>
+      <c r="L60" s="94"/>
+      <c r="M60" s="94"/>
+      <c r="N60" s="95">
+        <f>SUM(N49:N59)</f>
+        <v>24.75</v>
+      </c>
+      <c r="O60" s="95">
+        <f>SUM(O49:O59)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="23">
         <v>6</v>
       </c>
-      <c r="B57" s="77">
+      <c r="B61" s="74">
+        <v>42352</v>
+      </c>
+      <c r="C61" s="92" t="s">
+        <v>61</v>
+      </c>
+      <c r="D61" s="47">
+        <v>0.5</v>
+      </c>
+      <c r="E61" s="47"/>
+      <c r="F61" s="37">
+        <v>1</v>
+      </c>
+      <c r="G61" s="37"/>
+      <c r="H61" s="48">
+        <v>0.5</v>
+      </c>
+      <c r="I61" s="48"/>
+      <c r="J61" s="37">
+        <v>0.5</v>
+      </c>
+      <c r="K61" s="29"/>
+      <c r="L61" s="46"/>
+      <c r="M61" s="46"/>
+      <c r="N61" s="28">
+        <f t="shared" ref="N61:O68" si="39">D61+F61+H61+J61+L61</f>
+        <v>2.5</v>
+      </c>
+      <c r="O61" s="29">
+        <f t="shared" si="39"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="64">
+        <v>6</v>
+      </c>
+      <c r="B62" s="77">
         <v>42354</v>
       </c>
-      <c r="C57" s="55" t="s">
+      <c r="C62" s="55" t="s">
         <v>61</v>
       </c>
-      <c r="D57" s="47">
-        <v>0.5</v>
-      </c>
-      <c r="E57" s="47"/>
-      <c r="F57" s="37">
-        <v>1</v>
-      </c>
-      <c r="G57" s="37"/>
-      <c r="H57" s="48">
-        <v>0.5</v>
-      </c>
-      <c r="I57" s="48"/>
-      <c r="J57" s="37">
-        <v>0.5</v>
-      </c>
-      <c r="K57" s="97"/>
-      <c r="L57" s="98"/>
-      <c r="M57" s="98"/>
-      <c r="N57" s="99">
-        <f t="shared" ref="N57:N58" si="36">D57+F57+H57+J57+L57</f>
+      <c r="D62" s="47">
+        <v>0.5</v>
+      </c>
+      <c r="E62" s="47"/>
+      <c r="F62" s="37">
+        <v>1</v>
+      </c>
+      <c r="G62" s="37"/>
+      <c r="H62" s="48">
+        <v>0.5</v>
+      </c>
+      <c r="I62" s="48"/>
+      <c r="J62" s="37">
+        <v>0.5</v>
+      </c>
+      <c r="K62" s="97"/>
+      <c r="L62" s="98"/>
+      <c r="M62" s="98"/>
+      <c r="N62" s="99">
+        <f t="shared" ref="N62:N63" si="40">D62+F62+H62+J62+L62</f>
         <v>2.5</v>
       </c>
-      <c r="O57" s="97">
-        <f t="shared" ref="O57:O58" si="37">E57+G57+I57+K57+M57</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="30">
+      <c r="O62" s="97">
+        <f t="shared" ref="O62:O63" si="41">E62+G62+I62+K62+M62</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="30">
         <v>6</v>
       </c>
-      <c r="B58" s="75"/>
-      <c r="C58" s="55" t="s">
+      <c r="B63" s="75"/>
+      <c r="C63" s="55" t="s">
         <v>25</v>
       </c>
-      <c r="D58" s="51"/>
-      <c r="E58" s="51"/>
-      <c r="F58" s="30"/>
-      <c r="G58" s="30"/>
-      <c r="H58" s="52"/>
-      <c r="I58" s="52"/>
-      <c r="J58" s="30"/>
-      <c r="K58" s="30"/>
-      <c r="L58" s="49"/>
-      <c r="M58" s="49"/>
-      <c r="N58" s="36">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="O58" s="37">
-        <f t="shared" si="37"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="30">
+      <c r="D63" s="51"/>
+      <c r="E63" s="51"/>
+      <c r="F63" s="30"/>
+      <c r="G63" s="30"/>
+      <c r="H63" s="52"/>
+      <c r="I63" s="52"/>
+      <c r="J63" s="30"/>
+      <c r="K63" s="30"/>
+      <c r="L63" s="49"/>
+      <c r="M63" s="49"/>
+      <c r="N63" s="36">
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
+      <c r="O63" s="37">
+        <f t="shared" si="41"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="30">
         <v>6</v>
       </c>
-      <c r="B59" s="75"/>
-      <c r="C59" s="31"/>
-      <c r="D59" s="51"/>
-      <c r="E59" s="51"/>
-      <c r="F59" s="30"/>
-      <c r="G59" s="30"/>
-      <c r="H59" s="52"/>
-      <c r="I59" s="52"/>
-      <c r="J59" s="30"/>
-      <c r="K59" s="30"/>
-      <c r="L59" s="49"/>
-      <c r="M59" s="49"/>
-      <c r="N59" s="36">
-        <f t="shared" si="35"/>
-        <v>0</v>
-      </c>
-      <c r="O59" s="37">
-        <f t="shared" si="35"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="30">
+      <c r="B64" s="75"/>
+      <c r="C64" s="31"/>
+      <c r="D64" s="51"/>
+      <c r="E64" s="51"/>
+      <c r="F64" s="30"/>
+      <c r="G64" s="30"/>
+      <c r="H64" s="52"/>
+      <c r="I64" s="52"/>
+      <c r="J64" s="30"/>
+      <c r="K64" s="30"/>
+      <c r="L64" s="49"/>
+      <c r="M64" s="49"/>
+      <c r="N64" s="36">
+        <f t="shared" si="39"/>
+        <v>0</v>
+      </c>
+      <c r="O64" s="37">
+        <f t="shared" si="39"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="30">
         <v>6</v>
       </c>
-      <c r="B60" s="75"/>
-      <c r="C60" s="31"/>
-      <c r="D60" s="51"/>
-      <c r="E60" s="51"/>
-      <c r="F60" s="30"/>
-      <c r="G60" s="30"/>
-      <c r="H60" s="52"/>
-      <c r="I60" s="52"/>
-      <c r="J60" s="30"/>
-      <c r="K60" s="30"/>
-      <c r="L60" s="49"/>
-      <c r="M60" s="49"/>
-      <c r="N60" s="36">
-        <f t="shared" si="35"/>
-        <v>0</v>
-      </c>
-      <c r="O60" s="37">
-        <f t="shared" si="35"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="30">
+      <c r="B65" s="75"/>
+      <c r="C65" s="31"/>
+      <c r="D65" s="51"/>
+      <c r="E65" s="51"/>
+      <c r="F65" s="30"/>
+      <c r="G65" s="30"/>
+      <c r="H65" s="52"/>
+      <c r="I65" s="52"/>
+      <c r="J65" s="30"/>
+      <c r="K65" s="30"/>
+      <c r="L65" s="49"/>
+      <c r="M65" s="49"/>
+      <c r="N65" s="36">
+        <f t="shared" si="39"/>
+        <v>0</v>
+      </c>
+      <c r="O65" s="37">
+        <f t="shared" si="39"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="30">
         <v>6</v>
       </c>
-      <c r="B61" s="75"/>
-      <c r="C61" s="31"/>
-      <c r="D61" s="51"/>
-      <c r="E61" s="51"/>
-      <c r="F61" s="30"/>
-      <c r="G61" s="30"/>
-      <c r="H61" s="52"/>
-      <c r="I61" s="52"/>
-      <c r="J61" s="30"/>
-      <c r="K61" s="30"/>
-      <c r="L61" s="49"/>
-      <c r="M61" s="49"/>
-      <c r="N61" s="36">
-        <f t="shared" si="35"/>
-        <v>0</v>
-      </c>
-      <c r="O61" s="37">
-        <f t="shared" si="35"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="81">
-        <v>6</v>
-      </c>
-      <c r="B62" s="82"/>
-      <c r="C62" s="83"/>
-      <c r="D62" s="84"/>
-      <c r="E62" s="84"/>
-      <c r="F62" s="81"/>
-      <c r="G62" s="81"/>
-      <c r="H62" s="85"/>
-      <c r="I62" s="85"/>
-      <c r="J62" s="81"/>
-      <c r="K62" s="81"/>
-      <c r="L62" s="86"/>
-      <c r="M62" s="86"/>
-      <c r="N62" s="36">
-        <f t="shared" si="35"/>
-        <v>0</v>
-      </c>
-      <c r="O62" s="37">
-        <f t="shared" si="35"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="38">
-        <v>6</v>
-      </c>
-      <c r="B63" s="76">
-        <v>42358</v>
-      </c>
-      <c r="C63" s="69" t="s">
-        <v>29</v>
-      </c>
-      <c r="D63" s="40">
-        <v>0.25</v>
-      </c>
-      <c r="E63" s="40"/>
-      <c r="F63" s="62">
-        <v>0.25</v>
-      </c>
-      <c r="G63" s="62"/>
-      <c r="H63" s="42">
-        <v>0.25</v>
-      </c>
-      <c r="I63" s="42"/>
-      <c r="J63" s="41">
-        <v>0.25</v>
-      </c>
-      <c r="K63" s="41"/>
-      <c r="L63" s="50"/>
-      <c r="M63" s="50"/>
-      <c r="N63" s="44">
-        <f t="shared" si="35"/>
-        <v>1</v>
-      </c>
-      <c r="O63" s="45">
-        <f t="shared" si="35"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="104" t="s">
-        <v>43</v>
-      </c>
-      <c r="B64" s="104"/>
-      <c r="C64" s="104"/>
-      <c r="D64" s="104"/>
-      <c r="E64" s="104"/>
-      <c r="F64" s="104"/>
-      <c r="G64" s="104"/>
-      <c r="H64" s="104"/>
-      <c r="I64" s="104"/>
-      <c r="J64" s="104" t="s">
-        <v>49</v>
-      </c>
-      <c r="K64" s="105"/>
-      <c r="L64" s="94"/>
-      <c r="M64" s="94"/>
-      <c r="N64" s="95">
-        <f>SUM(N56:N63)</f>
-        <v>6</v>
-      </c>
-      <c r="O64" s="95">
-        <f>SUM(O56:O63)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="B65" s="74">
-        <v>42380</v>
-      </c>
-      <c r="C65" s="92" t="s">
-        <v>61</v>
-      </c>
-      <c r="D65" s="47">
-        <v>0.5</v>
-      </c>
-      <c r="E65" s="47"/>
-      <c r="F65" s="37">
-        <v>1</v>
-      </c>
-      <c r="G65" s="37"/>
-      <c r="H65" s="48">
-        <v>0.5</v>
-      </c>
-      <c r="I65" s="48"/>
-      <c r="J65" s="37">
-        <v>0.5</v>
-      </c>
-      <c r="K65" s="23"/>
-      <c r="L65" s="46"/>
-      <c r="M65" s="46"/>
-      <c r="N65" s="28">
-        <f t="shared" ref="N65:O70" si="38">D65+F65+H65+J65+L65</f>
-        <v>2.5</v>
-      </c>
-      <c r="O65" s="29">
-        <f t="shared" si="38"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="B66" s="75">
-        <v>42381</v>
-      </c>
-      <c r="C66" s="55" t="s">
-        <v>61</v>
-      </c>
-      <c r="D66" s="47">
-        <v>0.5</v>
-      </c>
-      <c r="E66" s="47"/>
-      <c r="F66" s="37">
-        <v>1</v>
-      </c>
-      <c r="G66" s="37"/>
-      <c r="H66" s="48">
-        <v>0.5</v>
-      </c>
-      <c r="I66" s="48"/>
-      <c r="J66" s="37">
-        <v>0.5</v>
-      </c>
+      <c r="B66" s="75"/>
+      <c r="C66" s="31"/>
+      <c r="D66" s="51"/>
+      <c r="E66" s="51"/>
+      <c r="F66" s="30"/>
+      <c r="G66" s="30"/>
+      <c r="H66" s="52"/>
+      <c r="I66" s="52"/>
+      <c r="J66" s="30"/>
       <c r="K66" s="30"/>
       <c r="L66" s="49"/>
       <c r="M66" s="49"/>
       <c r="N66" s="36">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
+        <v>0</v>
+      </c>
+      <c r="O66" s="37">
+        <f t="shared" si="39"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="81">
+        <v>6</v>
+      </c>
+      <c r="B67" s="82"/>
+      <c r="C67" s="83"/>
+      <c r="D67" s="84"/>
+      <c r="E67" s="84"/>
+      <c r="F67" s="81"/>
+      <c r="G67" s="81"/>
+      <c r="H67" s="85"/>
+      <c r="I67" s="85"/>
+      <c r="J67" s="81"/>
+      <c r="K67" s="81"/>
+      <c r="L67" s="86"/>
+      <c r="M67" s="86"/>
+      <c r="N67" s="36">
+        <f t="shared" si="39"/>
+        <v>0</v>
+      </c>
+      <c r="O67" s="37">
+        <f t="shared" si="39"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="38">
+        <v>6</v>
+      </c>
+      <c r="B68" s="76">
+        <v>42358</v>
+      </c>
+      <c r="C68" s="69" t="s">
+        <v>29</v>
+      </c>
+      <c r="D68" s="40">
+        <v>0.25</v>
+      </c>
+      <c r="E68" s="40"/>
+      <c r="F68" s="62">
+        <v>0.25</v>
+      </c>
+      <c r="G68" s="62"/>
+      <c r="H68" s="42">
+        <v>0.25</v>
+      </c>
+      <c r="I68" s="42"/>
+      <c r="J68" s="41">
+        <v>0.25</v>
+      </c>
+      <c r="K68" s="41"/>
+      <c r="L68" s="50"/>
+      <c r="M68" s="50"/>
+      <c r="N68" s="44">
+        <f t="shared" si="39"/>
+        <v>1</v>
+      </c>
+      <c r="O68" s="45">
+        <f t="shared" si="39"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="105" t="s">
+        <v>43</v>
+      </c>
+      <c r="B69" s="105"/>
+      <c r="C69" s="105"/>
+      <c r="D69" s="105"/>
+      <c r="E69" s="105"/>
+      <c r="F69" s="105"/>
+      <c r="G69" s="105"/>
+      <c r="H69" s="105"/>
+      <c r="I69" s="105"/>
+      <c r="J69" s="105" t="s">
+        <v>49</v>
+      </c>
+      <c r="K69" s="104"/>
+      <c r="L69" s="94"/>
+      <c r="M69" s="94"/>
+      <c r="N69" s="95">
+        <f>SUM(N61:N68)</f>
+        <v>6</v>
+      </c>
+      <c r="O69" s="95">
+        <f>SUM(O61:O68)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="B70" s="74">
+        <v>42380</v>
+      </c>
+      <c r="C70" s="92" t="s">
+        <v>61</v>
+      </c>
+      <c r="D70" s="47">
+        <v>0.5</v>
+      </c>
+      <c r="E70" s="47"/>
+      <c r="F70" s="37">
+        <v>1</v>
+      </c>
+      <c r="G70" s="37"/>
+      <c r="H70" s="48">
+        <v>0.5</v>
+      </c>
+      <c r="I70" s="48"/>
+      <c r="J70" s="37">
+        <v>0.5</v>
+      </c>
+      <c r="K70" s="23"/>
+      <c r="L70" s="46"/>
+      <c r="M70" s="46"/>
+      <c r="N70" s="28">
+        <f t="shared" ref="N70:O75" si="42">D70+F70+H70+J70+L70</f>
         <v>2.5</v>
       </c>
-      <c r="O66" s="37">
-        <f t="shared" si="38"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="30" t="s">
+      <c r="O70" s="29">
+        <f t="shared" si="42"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="B67" s="75">
+      <c r="B71" s="75">
+        <v>42381</v>
+      </c>
+      <c r="C71" s="55" t="s">
+        <v>61</v>
+      </c>
+      <c r="D71" s="47">
+        <v>0.5</v>
+      </c>
+      <c r="E71" s="47"/>
+      <c r="F71" s="37">
+        <v>1</v>
+      </c>
+      <c r="G71" s="37"/>
+      <c r="H71" s="48">
+        <v>0.5</v>
+      </c>
+      <c r="I71" s="48"/>
+      <c r="J71" s="37">
+        <v>0.5</v>
+      </c>
+      <c r="K71" s="30"/>
+      <c r="L71" s="49"/>
+      <c r="M71" s="49"/>
+      <c r="N71" s="36">
+        <f t="shared" si="42"/>
+        <v>2.5</v>
+      </c>
+      <c r="O71" s="37">
+        <f t="shared" si="42"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A72" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="B72" s="75">
         <v>42382</v>
       </c>
-      <c r="C67" s="100" t="s">
-        <v>61</v>
-      </c>
-      <c r="D67" s="47">
-        <v>0.5</v>
-      </c>
-      <c r="E67" s="47"/>
-      <c r="F67" s="37">
-        <v>1</v>
-      </c>
-      <c r="G67" s="37"/>
-      <c r="H67" s="48">
-        <v>0.5</v>
-      </c>
-      <c r="I67" s="48"/>
-      <c r="J67" s="37">
-        <v>0.5</v>
-      </c>
-      <c r="K67" s="30"/>
-      <c r="L67" s="49"/>
-      <c r="M67" s="49"/>
-      <c r="N67" s="36">
-        <f t="shared" si="38"/>
-        <v>2.5</v>
-      </c>
-      <c r="O67" s="37">
-        <f t="shared" si="38"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A68" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="B68" s="75">
-        <v>42383</v>
-      </c>
-      <c r="C68" s="100" t="s">
-        <v>61</v>
-      </c>
-      <c r="D68" s="47">
-        <v>0.5</v>
-      </c>
-      <c r="E68" s="47"/>
-      <c r="F68" s="37">
-        <v>1</v>
-      </c>
-      <c r="G68" s="37"/>
-      <c r="H68" s="48">
-        <v>0.5</v>
-      </c>
-      <c r="I68" s="48"/>
-      <c r="J68" s="37">
-        <v>0.5</v>
-      </c>
-      <c r="K68" s="30"/>
-      <c r="L68" s="49"/>
-      <c r="M68" s="49"/>
-      <c r="N68" s="36">
-        <f t="shared" si="38"/>
-        <v>2.5</v>
-      </c>
-      <c r="O68" s="37">
-        <f t="shared" si="38"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A69" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="B69" s="75">
-        <v>42384</v>
-      </c>
-      <c r="C69" s="55" t="s">
-        <v>61</v>
-      </c>
-      <c r="D69" s="47">
-        <v>0.5</v>
-      </c>
-      <c r="E69" s="47"/>
-      <c r="F69" s="37">
-        <v>1</v>
-      </c>
-      <c r="G69" s="37"/>
-      <c r="H69" s="48">
-        <v>0.5</v>
-      </c>
-      <c r="I69" s="48"/>
-      <c r="J69" s="37">
-        <v>0.5</v>
-      </c>
-      <c r="K69" s="30"/>
-      <c r="L69" s="49"/>
-      <c r="M69" s="49"/>
-      <c r="N69" s="36">
-        <f t="shared" si="38"/>
-        <v>2.5</v>
-      </c>
-      <c r="O69" s="37">
-        <f t="shared" si="38"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A70" s="38" t="s">
-        <v>8</v>
-      </c>
-      <c r="B70" s="76"/>
-      <c r="C70" s="39"/>
-      <c r="D70" s="53"/>
-      <c r="E70" s="53"/>
-      <c r="F70" s="38"/>
-      <c r="G70" s="38"/>
-      <c r="H70" s="54"/>
-      <c r="I70" s="54"/>
-      <c r="J70" s="38"/>
-      <c r="K70" s="38"/>
-      <c r="L70" s="50"/>
-      <c r="M70" s="50"/>
-      <c r="N70" s="44">
-        <f t="shared" si="38"/>
-        <v>0</v>
-      </c>
-      <c r="O70" s="45">
-        <f t="shared" si="38"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A71" s="104" t="s">
-        <v>44</v>
-      </c>
-      <c r="B71" s="104"/>
-      <c r="C71" s="104"/>
-      <c r="D71" s="104"/>
-      <c r="E71" s="104"/>
-      <c r="F71" s="104"/>
-      <c r="G71" s="104"/>
-      <c r="H71" s="104"/>
-      <c r="I71" s="104"/>
-      <c r="J71" s="104" t="s">
-        <v>50</v>
-      </c>
-      <c r="K71" s="105"/>
-      <c r="L71" s="94"/>
-      <c r="M71" s="94"/>
-      <c r="N71" s="95">
-        <f>SUM(N65:N70)</f>
-        <v>12.5</v>
-      </c>
-      <c r="O71" s="95">
-        <f>SUM(O65:O70)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A72" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="B72" s="74">
-        <v>42387</v>
-      </c>
-      <c r="C72" s="92" t="s">
+      <c r="C72" s="100" t="s">
         <v>61</v>
       </c>
       <c r="D72" s="47">
@@ -3616,26 +3663,26 @@
       <c r="J72" s="37">
         <v>0.5</v>
       </c>
-      <c r="K72" s="23"/>
-      <c r="L72" s="46"/>
-      <c r="M72" s="46"/>
-      <c r="N72" s="28">
-        <f t="shared" ref="N72:O74" si="39">D72+F72+H72+J72+L72</f>
+      <c r="K72" s="30"/>
+      <c r="L72" s="49"/>
+      <c r="M72" s="49"/>
+      <c r="N72" s="36">
+        <f t="shared" si="42"/>
         <v>2.5</v>
       </c>
-      <c r="O72" s="29">
-        <f t="shared" si="39"/>
+      <c r="O72" s="37">
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A73" s="30" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B73" s="75">
-        <v>42388</v>
-      </c>
-      <c r="C73" s="55" t="s">
+        <v>42383</v>
+      </c>
+      <c r="C73" s="100" t="s">
         <v>61</v>
       </c>
       <c r="D73" s="47">
@@ -3657,22 +3704,22 @@
       <c r="L73" s="49"/>
       <c r="M73" s="49"/>
       <c r="N73" s="36">
-        <f t="shared" si="39"/>
+        <f t="shared" si="42"/>
         <v>2.5</v>
       </c>
       <c r="O73" s="37">
-        <f t="shared" si="39"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
     </row>
     <row r="74" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A74" s="30" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B74" s="75">
-        <v>42389</v>
-      </c>
-      <c r="C74" s="100" t="s">
+        <v>42384</v>
+      </c>
+      <c r="C74" s="55" t="s">
         <v>61</v>
       </c>
       <c r="D74" s="47">
@@ -3694,222 +3741,401 @@
       <c r="L74" s="49"/>
       <c r="M74" s="49"/>
       <c r="N74" s="36">
-        <f t="shared" si="39"/>
+        <f t="shared" si="42"/>
         <v>2.5</v>
       </c>
       <c r="O74" s="37">
-        <f t="shared" si="39"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A75" s="30" t="s">
+      <c r="A75" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="B75" s="76"/>
+      <c r="C75" s="39"/>
+      <c r="D75" s="53"/>
+      <c r="E75" s="53"/>
+      <c r="F75" s="38"/>
+      <c r="G75" s="38"/>
+      <c r="H75" s="54"/>
+      <c r="I75" s="54"/>
+      <c r="J75" s="38"/>
+      <c r="K75" s="38"/>
+      <c r="L75" s="50"/>
+      <c r="M75" s="50"/>
+      <c r="N75" s="44">
+        <f t="shared" si="42"/>
+        <v>0</v>
+      </c>
+      <c r="O75" s="45">
+        <f t="shared" si="42"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A76" s="105" t="s">
+        <v>44</v>
+      </c>
+      <c r="B76" s="105"/>
+      <c r="C76" s="105"/>
+      <c r="D76" s="105"/>
+      <c r="E76" s="105"/>
+      <c r="F76" s="105"/>
+      <c r="G76" s="105"/>
+      <c r="H76" s="105"/>
+      <c r="I76" s="105"/>
+      <c r="J76" s="105" t="s">
+        <v>50</v>
+      </c>
+      <c r="K76" s="104"/>
+      <c r="L76" s="94"/>
+      <c r="M76" s="94"/>
+      <c r="N76" s="95">
+        <f>SUM(N70:N75)</f>
+        <v>12.5</v>
+      </c>
+      <c r="O76" s="95">
+        <f>SUM(O70:O75)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A77" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="B75" s="75">
+      <c r="B77" s="74">
+        <v>42387</v>
+      </c>
+      <c r="C77" s="92" t="s">
+        <v>61</v>
+      </c>
+      <c r="D77" s="47">
+        <v>0.5</v>
+      </c>
+      <c r="E77" s="47"/>
+      <c r="F77" s="37">
+        <v>1</v>
+      </c>
+      <c r="G77" s="37"/>
+      <c r="H77" s="48">
+        <v>0.5</v>
+      </c>
+      <c r="I77" s="48"/>
+      <c r="J77" s="37">
+        <v>0.5</v>
+      </c>
+      <c r="K77" s="23"/>
+      <c r="L77" s="46"/>
+      <c r="M77" s="46"/>
+      <c r="N77" s="28">
+        <f t="shared" ref="N77:O79" si="43">D77+F77+H77+J77+L77</f>
+        <v>2.5</v>
+      </c>
+      <c r="O77" s="29">
+        <f t="shared" si="43"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A78" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="B78" s="75">
+        <v>42388</v>
+      </c>
+      <c r="C78" s="55" t="s">
+        <v>61</v>
+      </c>
+      <c r="D78" s="47">
+        <v>0.5</v>
+      </c>
+      <c r="E78" s="47"/>
+      <c r="F78" s="37">
+        <v>1</v>
+      </c>
+      <c r="G78" s="37"/>
+      <c r="H78" s="48">
+        <v>0.5</v>
+      </c>
+      <c r="I78" s="48"/>
+      <c r="J78" s="37">
+        <v>0.5</v>
+      </c>
+      <c r="K78" s="30"/>
+      <c r="L78" s="49"/>
+      <c r="M78" s="49"/>
+      <c r="N78" s="36">
+        <f t="shared" si="43"/>
+        <v>2.5</v>
+      </c>
+      <c r="O78" s="37">
+        <f t="shared" si="43"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A79" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="B79" s="75">
+        <v>42389</v>
+      </c>
+      <c r="C79" s="100" t="s">
+        <v>61</v>
+      </c>
+      <c r="D79" s="47">
+        <v>0.5</v>
+      </c>
+      <c r="E79" s="47"/>
+      <c r="F79" s="37">
+        <v>1</v>
+      </c>
+      <c r="G79" s="37"/>
+      <c r="H79" s="48">
+        <v>0.5</v>
+      </c>
+      <c r="I79" s="48"/>
+      <c r="J79" s="37">
+        <v>0.5</v>
+      </c>
+      <c r="K79" s="30"/>
+      <c r="L79" s="49"/>
+      <c r="M79" s="49"/>
+      <c r="N79" s="36">
+        <f t="shared" si="43"/>
+        <v>2.5</v>
+      </c>
+      <c r="O79" s="37">
+        <f t="shared" si="43"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A80" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="B80" s="75">
         <v>42390</v>
       </c>
-      <c r="C75" s="100" t="s">
+      <c r="C80" s="100" t="s">
         <v>61</v>
       </c>
-      <c r="D75" s="47">
-        <v>0.5</v>
-      </c>
-      <c r="E75" s="47"/>
-      <c r="F75" s="37">
-        <v>1</v>
-      </c>
-      <c r="G75" s="37"/>
-      <c r="H75" s="48">
-        <v>0.5</v>
-      </c>
-      <c r="I75" s="48"/>
-      <c r="J75" s="37">
-        <v>0.5</v>
-      </c>
-      <c r="K75" s="30"/>
-      <c r="L75" s="49"/>
-      <c r="M75" s="49"/>
-      <c r="N75" s="36">
-        <f t="shared" ref="N75:N78" si="40">D75+F75+H75+J75+L75</f>
+      <c r="D80" s="47">
+        <v>0.5</v>
+      </c>
+      <c r="E80" s="47"/>
+      <c r="F80" s="37">
+        <v>1</v>
+      </c>
+      <c r="G80" s="37"/>
+      <c r="H80" s="48">
+        <v>0.5</v>
+      </c>
+      <c r="I80" s="48"/>
+      <c r="J80" s="37">
+        <v>0.5</v>
+      </c>
+      <c r="K80" s="30"/>
+      <c r="L80" s="49"/>
+      <c r="M80" s="49"/>
+      <c r="N80" s="36">
+        <f t="shared" ref="N80:N83" si="44">D80+F80+H80+J80+L80</f>
         <v>2.5</v>
       </c>
-      <c r="O75" s="37">
-        <f t="shared" ref="O75:O78" si="41">E75+G75+I75+K75+M75</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A76" s="30" t="s">
+      <c r="O80" s="37">
+        <f t="shared" ref="O80:O83" si="45">E80+G80+I80+K80+M80</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A81" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="B76" s="75">
+      <c r="B81" s="75">
         <v>42391</v>
       </c>
-      <c r="C76" s="55" t="s">
+      <c r="C81" s="55" t="s">
         <v>61</v>
       </c>
-      <c r="D76" s="47">
-        <v>0.5</v>
-      </c>
-      <c r="E76" s="47"/>
-      <c r="F76" s="37">
-        <v>1</v>
-      </c>
-      <c r="G76" s="37"/>
-      <c r="H76" s="48">
-        <v>0.5</v>
-      </c>
-      <c r="I76" s="48"/>
-      <c r="J76" s="37">
-        <v>0.5</v>
-      </c>
-      <c r="K76" s="30"/>
-      <c r="L76" s="49"/>
-      <c r="M76" s="49"/>
-      <c r="N76" s="36">
-        <f t="shared" si="40"/>
+      <c r="D81" s="47">
+        <v>0.5</v>
+      </c>
+      <c r="E81" s="47"/>
+      <c r="F81" s="37">
+        <v>1</v>
+      </c>
+      <c r="G81" s="37"/>
+      <c r="H81" s="48">
+        <v>0.5</v>
+      </c>
+      <c r="I81" s="48"/>
+      <c r="J81" s="37">
+        <v>0.5</v>
+      </c>
+      <c r="K81" s="30"/>
+      <c r="L81" s="49"/>
+      <c r="M81" s="49"/>
+      <c r="N81" s="36">
+        <f t="shared" si="44"/>
         <v>2.5</v>
       </c>
-      <c r="O76" s="37">
-        <f t="shared" si="41"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A77" s="30" t="s">
+      <c r="O81" s="37">
+        <f t="shared" si="45"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A82" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="B77" s="82"/>
-      <c r="C77" s="88"/>
-      <c r="D77" s="84"/>
-      <c r="E77" s="84"/>
-      <c r="F77" s="81"/>
-      <c r="G77" s="81"/>
-      <c r="H77" s="85"/>
-      <c r="I77" s="85"/>
-      <c r="J77" s="81"/>
-      <c r="K77" s="81"/>
-      <c r="L77" s="86"/>
-      <c r="M77" s="86"/>
-      <c r="N77" s="101">
-        <f t="shared" si="40"/>
-        <v>0</v>
-      </c>
-      <c r="O77" s="87">
-        <f t="shared" si="41"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A78" s="38"/>
-      <c r="B78" s="76">
+      <c r="B82" s="82"/>
+      <c r="C82" s="88"/>
+      <c r="D82" s="84"/>
+      <c r="E82" s="84"/>
+      <c r="F82" s="81"/>
+      <c r="G82" s="81"/>
+      <c r="H82" s="85"/>
+      <c r="I82" s="85"/>
+      <c r="J82" s="81"/>
+      <c r="K82" s="81"/>
+      <c r="L82" s="86"/>
+      <c r="M82" s="86"/>
+      <c r="N82" s="101">
+        <f t="shared" si="44"/>
+        <v>0</v>
+      </c>
+      <c r="O82" s="87">
+        <f t="shared" si="45"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A83" s="38"/>
+      <c r="B83" s="76">
         <v>42393</v>
       </c>
-      <c r="C78" s="69" t="s">
+      <c r="C83" s="69" t="s">
         <v>57</v>
       </c>
-      <c r="D78" s="53"/>
-      <c r="E78" s="53"/>
-      <c r="F78" s="38"/>
-      <c r="G78" s="38"/>
-      <c r="H78" s="54"/>
-      <c r="I78" s="54"/>
-      <c r="J78" s="38"/>
-      <c r="K78" s="38"/>
-      <c r="L78" s="50"/>
-      <c r="M78" s="50"/>
-      <c r="N78" s="44">
-        <f t="shared" si="40"/>
-        <v>0</v>
-      </c>
-      <c r="O78" s="45">
-        <f t="shared" si="41"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A79" s="3"/>
-      <c r="B79" s="78"/>
-      <c r="C79" s="3"/>
-      <c r="D79" s="6"/>
-      <c r="E79" s="6"/>
-      <c r="F79" s="3"/>
-      <c r="G79" s="3"/>
-      <c r="H79" s="5"/>
-      <c r="I79" s="5"/>
-      <c r="J79" s="104" t="s">
+      <c r="D83" s="53"/>
+      <c r="E83" s="53"/>
+      <c r="F83" s="38"/>
+      <c r="G83" s="38"/>
+      <c r="H83" s="54"/>
+      <c r="I83" s="54"/>
+      <c r="J83" s="38"/>
+      <c r="K83" s="38"/>
+      <c r="L83" s="50"/>
+      <c r="M83" s="50"/>
+      <c r="N83" s="44">
+        <f t="shared" si="44"/>
+        <v>0</v>
+      </c>
+      <c r="O83" s="45">
+        <f t="shared" si="45"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A84" s="3"/>
+      <c r="B84" s="78"/>
+      <c r="C84" s="3"/>
+      <c r="D84" s="6"/>
+      <c r="E84" s="6"/>
+      <c r="F84" s="3"/>
+      <c r="G84" s="3"/>
+      <c r="H84" s="5"/>
+      <c r="I84" s="5"/>
+      <c r="J84" s="105" t="s">
         <v>51</v>
       </c>
-      <c r="K79" s="105"/>
-      <c r="L79" s="2"/>
-      <c r="M79" s="2"/>
-      <c r="N79" s="8">
-        <f>SUM(N72:N78)</f>
+      <c r="K84" s="104"/>
+      <c r="L84" s="2"/>
+      <c r="M84" s="2"/>
+      <c r="N84" s="8">
+        <f>SUM(N77:N83)</f>
         <v>12.5</v>
       </c>
-      <c r="O79" s="4">
-        <f>SUM(O72:O78)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A80" s="9"/>
-      <c r="B80" s="79"/>
-      <c r="C80" s="10" t="s">
+      <c r="O84" s="4">
+        <f>SUM(O77:O83)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A85" s="9"/>
+      <c r="B85" s="79"/>
+      <c r="C85" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D80" s="11">
-        <f t="shared" ref="D80:M80" si="42">SUM(D4:D79)</f>
-        <v>41.75</v>
-      </c>
-      <c r="E80" s="11">
-        <f t="shared" si="42"/>
-        <v>34.75</v>
-      </c>
-      <c r="F80" s="11">
-        <f t="shared" si="42"/>
-        <v>47</v>
-      </c>
-      <c r="G80" s="11">
-        <f t="shared" si="42"/>
-        <v>33.5</v>
-      </c>
-      <c r="H80" s="11">
-        <f t="shared" si="42"/>
-        <v>38.5</v>
-      </c>
-      <c r="I80" s="11">
-        <f t="shared" si="42"/>
-        <v>30</v>
-      </c>
-      <c r="J80" s="11">
-        <f t="shared" si="42"/>
-        <v>41.5</v>
-      </c>
-      <c r="K80" s="11">
-        <f t="shared" si="42"/>
-        <v>35.5</v>
-      </c>
-      <c r="L80" s="11">
-        <f t="shared" si="42"/>
-        <v>0.5</v>
-      </c>
-      <c r="M80" s="11">
-        <f t="shared" si="42"/>
-        <v>0.5</v>
-      </c>
-      <c r="N80" s="9">
-        <f>D80+F80+H80+J80+L80</f>
-        <v>169.25</v>
-      </c>
-      <c r="O80" s="11">
-        <f>E80+G80+I80+K80+M80</f>
-        <v>134.25</v>
+      <c r="D85" s="11">
+        <f t="shared" ref="D85:M85" si="46">SUM(D4:D84)</f>
+        <v>46.5</v>
+      </c>
+      <c r="E85" s="11">
+        <f t="shared" si="46"/>
+        <v>40</v>
+      </c>
+      <c r="F85" s="11">
+        <f t="shared" si="46"/>
+        <v>51.25</v>
+      </c>
+      <c r="G85" s="11">
+        <f t="shared" si="46"/>
+        <v>36.5</v>
+      </c>
+      <c r="H85" s="11">
+        <f t="shared" si="46"/>
+        <v>43.25</v>
+      </c>
+      <c r="I85" s="11">
+        <f t="shared" si="46"/>
+        <v>32</v>
+      </c>
+      <c r="J85" s="11">
+        <f t="shared" si="46"/>
+        <v>46.25</v>
+      </c>
+      <c r="K85" s="11">
+        <f t="shared" si="46"/>
+        <v>39</v>
+      </c>
+      <c r="L85" s="11">
+        <f t="shared" si="46"/>
+        <v>0.5</v>
+      </c>
+      <c r="M85" s="11">
+        <f t="shared" si="46"/>
+        <v>0.5</v>
+      </c>
+      <c r="N85" s="9">
+        <f>D85+F85+H85+J85+L85</f>
+        <v>187.75</v>
+      </c>
+      <c r="O85" s="11">
+        <f>E85+G85+I85+K85+M85</f>
+        <v>148</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="J84:K84"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="A5:I5"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="A60:I60"/>
+    <mergeCell ref="J60:K60"/>
+    <mergeCell ref="A69:I69"/>
+    <mergeCell ref="J69:K69"/>
+    <mergeCell ref="A76:I76"/>
+    <mergeCell ref="J76:K76"/>
+    <mergeCell ref="A22:I22"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="A36:I36"/>
+    <mergeCell ref="J36:K36"/>
+    <mergeCell ref="A48:I48"/>
+    <mergeCell ref="J48:K48"/>
     <mergeCell ref="J11:K11"/>
     <mergeCell ref="A11:I11"/>
     <mergeCell ref="E2:F2"/>
@@ -3918,22 +4144,6 @@
     <mergeCell ref="F4:G4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="J4:K4"/>
-    <mergeCell ref="J79:K79"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="A5:I5"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="A55:I55"/>
-    <mergeCell ref="J55:K55"/>
-    <mergeCell ref="A64:I64"/>
-    <mergeCell ref="J64:K64"/>
-    <mergeCell ref="A71:I71"/>
-    <mergeCell ref="J71:K71"/>
-    <mergeCell ref="A22:I22"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="A36:I36"/>
-    <mergeCell ref="J36:K36"/>
-    <mergeCell ref="A47:I47"/>
-    <mergeCell ref="J47:K47"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.55118110236220474" right="0.55118110236220474" top="0.39370078740157483" bottom="0.39370078740157483" header="0.51181102362204722" footer="0.51181102362204722"/>
@@ -3959,29 +4169,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement>
-    <Volgorde_x0020_Documenten xmlns="9ab5e87a-ed8e-45a5-9793-059f67398425">6</Volgorde_x0020_Documenten>
-    <Categorie xmlns="9ab5e87a-ed8e-45a5-9793-059f67398425">Extra</Categorie>
-    <Week xmlns="9ab5e87a-ed8e-45a5-9793-059f67398425">Geen week</Week>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008D777D35650D3B43A23D41664AA30BC5" ma:contentTypeVersion="" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="7f80e5700d93aba1c148b391c267eb5e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9ab5e87a-ed8e-45a5-9793-059f67398425" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e36a552b910c1cdf142adc90bba5ebe9" ns2:_="">
     <xsd:import namespace="9ab5e87a-ed8e-45a5-9793-059f67398425"/>
@@ -4142,15 +4329,56 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement>
+    <Volgorde_x0020_Documenten xmlns="9ab5e87a-ed8e-45a5-9793-059f67398425">6</Volgorde_x0020_Documenten>
+    <Categorie xmlns="9ab5e87a-ed8e-45a5-9793-059f67398425">Extra</Categorie>
+    <Week xmlns="9ab5e87a-ed8e-45a5-9793-059f67398425">Geen week</Week>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1278A3E-47B6-4321-AA7E-C8551E08DBCA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C6B4BC2B-47EC-4A4E-997D-A663CFE6E409}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="9ab5e87a-ed8e-45a5-9793-059f67398425"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7925AB61-19A0-4A39-BC21-6A09D18176D2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D152C796-12D2-40E1-BE4C-837EB7333423}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -4166,28 +4394,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7925AB61-19A0-4A39-BC21-6A09D18176D2}">
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1278A3E-47B6-4321-AA7E-C8551E08DBCA}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C6B4BC2B-47EC-4A4E-997D-A663CFE6E409}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="9ab5e87a-ed8e-45a5-9793-059f67398425"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>